<commit_message>
Subindo alterações no gráfico de GANTT
</commit_message>
<xml_diff>
--- a/Documentação/Gráficos/Gráfico de GANTT.xlsx
+++ b/Documentação/Gráficos/Gráfico de GANTT.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITHUB\Documentos\SPRINT2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITHUB\Documentos\Documentação\Gráficos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58952B11-E128-4B90-824E-CDA2256D9C82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69CBF6E2-3217-4098-9746-E7726354ACF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="461" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -545,11 +545,11 @@
     <xf numFmtId="14" fontId="9" fillId="8" borderId="5" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="15" fillId="8" borderId="5" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="8" borderId="5" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -564,27 +564,6 @@
     <cellStyle name="Saída" xfId="5" builtinId="21"/>
   </cellStyles>
   <dxfs count="25">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -708,6 +687,27 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -949,7 +949,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.10526315789473684</c:v>
+                  <c:v>0.36842105263157893</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3002,17 +3002,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C9">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="22" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="21" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10:F10">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="20" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3026,10 +3026,10 @@
   <dimension ref="A1:EQ24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="8" topLeftCell="H11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="8" topLeftCell="H12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9:C20"/>
+      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3064,7 +3064,7 @@
       <c r="G2" s="31"/>
     </row>
     <row r="4" spans="1:147" s="2" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="38" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="32" t="s">
@@ -3077,31 +3077,31 @@
       <c r="G4" s="35"/>
     </row>
     <row r="5" spans="1:147" s="2" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="37"/>
+      <c r="C5" s="38"/>
       <c r="D5" s="33" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="33"/>
       <c r="F5" s="36">
         <f ca="1">TODAY()</f>
-        <v>44654</v>
+        <v>44661</v>
       </c>
       <c r="G5" s="36"/>
     </row>
     <row r="6" spans="1:147" s="2" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="27">
         <f>(SUM(CÁLCULOS!A3:A22)/SUM('COM FÓRMULAS'!D9:D20))</f>
-        <v>0.10526315789473684</v>
+        <v>0.36842105263157893</v>
       </c>
       <c r="D6" s="34" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="34"/>
-      <c r="F6" s="38">
+      <c r="F6" s="37">
         <f>(F20-E9)+1</f>
         <v>25</v>
       </c>
-      <c r="G6" s="38"/>
+      <c r="G6" s="37"/>
     </row>
     <row r="7" spans="1:147" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H7" s="28">
@@ -4226,7 +4226,7 @@
         <v>44652</v>
       </c>
       <c r="G11" s="10">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H11" s="19"/>
       <c r="I11" s="19"/>
@@ -4709,7 +4709,7 @@
         <v>44663</v>
       </c>
       <c r="G14" s="10">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H14" s="19"/>
       <c r="I14" s="19"/>
@@ -4870,7 +4870,7 @@
         <v>44663</v>
       </c>
       <c r="G15" s="10">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="19"/>
@@ -5031,7 +5031,7 @@
         <v>44664</v>
       </c>
       <c r="G16" s="10">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="19"/>
@@ -5192,7 +5192,7 @@
         <v>44665</v>
       </c>
       <c r="G17" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="19"/>
@@ -5353,7 +5353,7 @@
         <v>44665</v>
       </c>
       <c r="G18" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="19"/>
@@ -5514,7 +5514,7 @@
         <v>44666</v>
       </c>
       <c r="G19" s="10">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H19" s="19"/>
       <c r="I19" s="19"/>
@@ -5674,7 +5674,7 @@
         <v>44669</v>
       </c>
       <c r="G20" s="10">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H20" s="19"/>
       <c r="I20" s="19"/>
@@ -5825,18 +5825,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="EK7:EQ7"/>
-    <mergeCell ref="BE7:BK7"/>
-    <mergeCell ref="BS7:BY7"/>
-    <mergeCell ref="BZ7:CF7"/>
-    <mergeCell ref="CG7:CM7"/>
-    <mergeCell ref="CN7:CT7"/>
-    <mergeCell ref="CU7:DA7"/>
-    <mergeCell ref="DB7:DH7"/>
-    <mergeCell ref="DI7:DO7"/>
-    <mergeCell ref="DP7:DV7"/>
-    <mergeCell ref="DW7:EC7"/>
-    <mergeCell ref="ED7:EJ7"/>
     <mergeCell ref="AX7:BD7"/>
     <mergeCell ref="BL7:BR7"/>
     <mergeCell ref="A1:G2"/>
@@ -5853,39 +5841,51 @@
     <mergeCell ref="AC7:AI7"/>
     <mergeCell ref="AJ7:AP7"/>
     <mergeCell ref="AQ7:AW7"/>
+    <mergeCell ref="EK7:EQ7"/>
+    <mergeCell ref="BE7:BK7"/>
+    <mergeCell ref="BS7:BY7"/>
+    <mergeCell ref="BZ7:CF7"/>
+    <mergeCell ref="CG7:CM7"/>
+    <mergeCell ref="CN7:CT7"/>
+    <mergeCell ref="CU7:DA7"/>
+    <mergeCell ref="DB7:DH7"/>
+    <mergeCell ref="DI7:DO7"/>
+    <mergeCell ref="DP7:DV7"/>
+    <mergeCell ref="DW7:EC7"/>
+    <mergeCell ref="ED7:EJ7"/>
   </mergeCells>
   <conditionalFormatting sqref="B18:D19 B17 D17 B9:G10 B16:D16 E16:F20 B11:F15 G11:G20">
-    <cfRule type="expression" dxfId="22" priority="20">
+    <cfRule type="expression" dxfId="19" priority="20">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:BD19 BL9:EQ19">
-    <cfRule type="expression" dxfId="21" priority="19">
+    <cfRule type="expression" dxfId="18" priority="19">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:BD19 BL9:EQ19">
-    <cfRule type="expression" dxfId="20" priority="17">
+    <cfRule type="expression" dxfId="17" priority="17">
       <formula>AND(H$8&gt;=$E9,H$8&lt;=$F9)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:BD19 BL9:EQ19">
-    <cfRule type="expression" dxfId="19" priority="18">
+    <cfRule type="expression" dxfId="16" priority="18">
       <formula>OR(WEEKDAY(H$8,2)=6,WEEKDAY(H$8,2)=7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE9:BK19">
-    <cfRule type="expression" dxfId="18" priority="15">
+    <cfRule type="expression" dxfId="15" priority="15">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE9:BK19">
-    <cfRule type="expression" dxfId="17" priority="13">
+    <cfRule type="expression" dxfId="14" priority="13">
       <formula>AND(BE$8&gt;=$E9,BE$8&lt;=$F9)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE9:BK19">
-    <cfRule type="expression" dxfId="16" priority="14">
+    <cfRule type="expression" dxfId="13" priority="14">
       <formula>OR(WEEKDAY(BE$8,2)=6,WEEKDAY(BE$8,2)=7)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5904,42 +5904,42 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:D20">
-    <cfRule type="expression" dxfId="15" priority="10">
+    <cfRule type="expression" dxfId="12" priority="10">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H20:BD20 BL20:EQ20">
-    <cfRule type="expression" dxfId="14" priority="9">
+    <cfRule type="expression" dxfId="11" priority="9">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H20:BD20 BL20:EQ20">
-    <cfRule type="expression" dxfId="13" priority="7">
+    <cfRule type="expression" dxfId="10" priority="7">
       <formula>AND(H$8&gt;=$E20,H$8&lt;=$F20)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H20:BD20 BL20:EQ20">
-    <cfRule type="expression" dxfId="12" priority="8">
+    <cfRule type="expression" dxfId="9" priority="8">
       <formula>OR(WEEKDAY(H$8,2)=6,WEEKDAY(H$8,2)=7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE20:BK20">
-    <cfRule type="expression" dxfId="11" priority="5">
+    <cfRule type="expression" dxfId="8" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE20:BK20">
-    <cfRule type="expression" dxfId="10" priority="3">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>AND(BE$8&gt;=$E20,BE$8&lt;=$F20)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE20:BK20">
-    <cfRule type="expression" dxfId="9" priority="4">
+    <cfRule type="expression" dxfId="6" priority="4">
       <formula>OR(WEEKDAY(BE$8,2)=6,WEEKDAY(BE$8,2)=7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6071,11 +6071,11 @@
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>'COM FÓRMULAS'!D11*'COM FÓRMULAS'!G11</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" s="23">
         <f>IFERROR(WORKDAY('COM FÓRMULAS'!E11,CÁLCULOS!A5-1),"-")</f>
-        <v>44650</v>
+        <v>44651</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -6101,41 +6101,41 @@
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <f>'COM FÓRMULAS'!D14*'COM FÓRMULAS'!G14</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B8" s="23">
         <f>IFERROR(WORKDAY('COM FÓRMULAS'!E14,CÁLCULOS!A8-1),"-")</f>
-        <v>44659</v>
+        <v>44662</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <f>'COM FÓRMULAS'!D15*'COM FÓRMULAS'!G15</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B9" s="23">
         <f>IFERROR(WORKDAY('COM FÓRMULAS'!E15,CÁLCULOS!A9-1),"-")</f>
-        <v>44659</v>
+        <v>44662</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>'COM FÓRMULAS'!D18*'COM FÓRMULAS'!G18</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B10" s="23">
         <f>IFERROR(WORKDAY('COM FÓRMULAS'!E18,CÁLCULOS!A10-1),"-")</f>
-        <v>44664</v>
+        <v>44665</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>'COM FÓRMULAS'!D20*'COM FÓRMULAS'!G20</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B11" s="23">
         <f>IFERROR(WORKDAY('COM FÓRMULAS'!E20,CÁLCULOS!A11-1),"-")</f>
-        <v>44666</v>
+        <v>44669</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Alterações na documentação, gráfico de GANTT e no PBC
</commit_message>
<xml_diff>
--- a/Documentação/Gráficos/Gráfico de GANTT.xlsx
+++ b/Documentação/Gráficos/Gráfico de GANTT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITHUB\Documentos\Documentação\Gráficos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69CBF6E2-3217-4098-9746-E7726354ACF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E99969E-EE82-448E-AEEF-EB210C4F3CE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="461" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -949,7 +949,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.36842105263157893</c:v>
+                  <c:v>0.57894736842105265</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3029,7 +3029,7 @@
       <pane xSplit="7" ySplit="8" topLeftCell="H12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomRight" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3084,14 +3084,14 @@
       <c r="E5" s="33"/>
       <c r="F5" s="36">
         <f ca="1">TODAY()</f>
-        <v>44661</v>
+        <v>44667</v>
       </c>
       <c r="G5" s="36"/>
     </row>
     <row r="6" spans="1:147" s="2" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="27">
         <f>(SUM(CÁLCULOS!A3:A22)/SUM('COM FÓRMULAS'!D9:D20))</f>
-        <v>0.36842105263157893</v>
+        <v>0.57894736842105265</v>
       </c>
       <c r="D6" s="34" t="s">
         <v>7</v>
@@ -4387,7 +4387,7 @@
         <v>44655</v>
       </c>
       <c r="G12" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="19"/>
       <c r="I12" s="19"/>
@@ -4548,7 +4548,7 @@
         <v>44659</v>
       </c>
       <c r="G13" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" s="19"/>
       <c r="I13" s="19"/>
@@ -4870,7 +4870,7 @@
         <v>44663</v>
       </c>
       <c r="G15" s="10">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="19"/>
@@ -5514,7 +5514,7 @@
         <v>44666</v>
       </c>
       <c r="G19" s="10">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H19" s="19"/>
       <c r="I19" s="19"/>
@@ -5825,6 +5825,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="EK7:EQ7"/>
+    <mergeCell ref="BE7:BK7"/>
+    <mergeCell ref="BS7:BY7"/>
+    <mergeCell ref="BZ7:CF7"/>
+    <mergeCell ref="CG7:CM7"/>
+    <mergeCell ref="CN7:CT7"/>
+    <mergeCell ref="CU7:DA7"/>
+    <mergeCell ref="DB7:DH7"/>
+    <mergeCell ref="DI7:DO7"/>
+    <mergeCell ref="DP7:DV7"/>
+    <mergeCell ref="DW7:EC7"/>
+    <mergeCell ref="ED7:EJ7"/>
     <mergeCell ref="AX7:BD7"/>
     <mergeCell ref="BL7:BR7"/>
     <mergeCell ref="A1:G2"/>
@@ -5841,18 +5853,6 @@
     <mergeCell ref="AC7:AI7"/>
     <mergeCell ref="AJ7:AP7"/>
     <mergeCell ref="AQ7:AW7"/>
-    <mergeCell ref="EK7:EQ7"/>
-    <mergeCell ref="BE7:BK7"/>
-    <mergeCell ref="BS7:BY7"/>
-    <mergeCell ref="BZ7:CF7"/>
-    <mergeCell ref="CG7:CM7"/>
-    <mergeCell ref="CN7:CT7"/>
-    <mergeCell ref="CU7:DA7"/>
-    <mergeCell ref="DB7:DH7"/>
-    <mergeCell ref="DI7:DO7"/>
-    <mergeCell ref="DP7:DV7"/>
-    <mergeCell ref="DW7:EC7"/>
-    <mergeCell ref="ED7:EJ7"/>
   </mergeCells>
   <conditionalFormatting sqref="B18:D19 B17 D17 B9:G10 B16:D16 E16:F20 B11:F15 G11:G20">
     <cfRule type="expression" dxfId="19" priority="20">
@@ -6081,21 +6081,21 @@
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <f>'COM FÓRMULAS'!D12*'COM FÓRMULAS'!G12</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6" s="23">
         <f>IFERROR(WORKDAY('COM FÓRMULAS'!E12,CÁLCULOS!A6-1),"-")</f>
-        <v>44652</v>
+        <v>44655</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>'COM FÓRMULAS'!D13*'COM FÓRMULAS'!G13</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B7" s="23">
         <f>IFERROR(WORKDAY('COM FÓRMULAS'!E13,CÁLCULOS!A7-1),"-")</f>
-        <v>44657</v>
+        <v>44659</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -6111,11 +6111,11 @@
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <f>'COM FÓRMULAS'!D15*'COM FÓRMULAS'!G15</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B9" s="23">
         <f>IFERROR(WORKDAY('COM FÓRMULAS'!E15,CÁLCULOS!A9-1),"-")</f>
-        <v>44662</v>
+        <v>44663</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Subindo alterações no gráfico de GANTT e na documentação do projeto
</commit_message>
<xml_diff>
--- a/Documentação/Gráficos/Gráfico de GANTT.xlsx
+++ b/Documentação/Gráficos/Gráfico de GANTT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITHUB\Documentos\Documentação\Gráficos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E99969E-EE82-448E-AEEF-EB210C4F3CE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367E3731-C23C-4A3B-82AD-E63FF2E267A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="461" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>#</t>
   </si>
@@ -100,6 +100,39 @@
   </si>
   <si>
     <t>Implementação de lista</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mínimo 4 Telas integradas- React </t>
+  </si>
+  <si>
+    <t>Planilha de UAT</t>
+  </si>
+  <si>
+    <t>Projeto WEB aderente com UX+UI</t>
+  </si>
+  <si>
+    <t>Documento de Layout de exportação</t>
+  </si>
+  <si>
+    <t>Exportação de dados para arquivo texto</t>
+  </si>
+  <si>
+    <t>Diagrama de solução de software - Componentes</t>
+  </si>
+  <si>
+    <t>Teste Unitário - API</t>
+  </si>
+  <si>
+    <t>Implementação de pilha</t>
+  </si>
+  <si>
+    <t>Documento de Layout de importação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Importação dos dados do arquivo texto </t>
+  </si>
+  <si>
+    <t>Testes unitários (Alinhado com Yoshi</t>
   </si>
 </sst>
 </file>
@@ -437,7 +470,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -551,6 +584,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Bom" xfId="2" builtinId="26"/>
@@ -563,7 +599,56 @@
     <cellStyle name="Ruim" xfId="3" builtinId="27"/>
     <cellStyle name="Saída" xfId="5" builtinId="21"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="31">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -732,13 +817,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -818,8 +896,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.25352007990151676"/>
-          <c:y val="0"/>
+          <c:x val="0.44004686109515279"/>
+          <c:y val="1.1185682326621925E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -949,7 +1027,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.57894736842105265</c:v>
+                  <c:v>0.34285714285714286</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1715,8 +1793,8 @@
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>68580</xdr:colOff>
+      <xdr:col>77</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
@@ -2015,7 +2093,7 @@
       <pane xSplit="7" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
+      <selection pane="bottomRight" activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2992,27 +3070,27 @@
     <mergeCell ref="AJ1:AP1"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:B10 D3:G9 D10 G10">
-    <cfRule type="expression" dxfId="24" priority="5">
+    <cfRule type="expression" dxfId="30" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:BK10">
-    <cfRule type="expression" dxfId="23" priority="4">
+    <cfRule type="expression" dxfId="29" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C9">
-    <cfRule type="expression" dxfId="22" priority="3">
+    <cfRule type="expression" dxfId="28" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="21" priority="2">
+    <cfRule type="expression" dxfId="27" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10:F10">
-    <cfRule type="expression" dxfId="20" priority="1">
+    <cfRule type="expression" dxfId="26" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3023,13 +3101,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:EQ24"/>
+  <dimension ref="A1:EQ35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="8" topLeftCell="H12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="8" topLeftCell="AV24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G20" sqref="G20"/>
+      <selection pane="bottomRight" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3084,22 +3162,22 @@
       <c r="E5" s="33"/>
       <c r="F5" s="36">
         <f ca="1">TODAY()</f>
-        <v>44667</v>
+        <v>44689</v>
       </c>
       <c r="G5" s="36"/>
     </row>
     <row r="6" spans="1:147" s="2" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="27">
-        <f>(SUM(CÁLCULOS!A3:A22)/SUM('COM FÓRMULAS'!D9:D20))</f>
-        <v>0.57894736842105265</v>
+        <f>(SUM(CÁLCULOS!A3:A22)/SUM('COM FÓRMULAS'!D9:D31))</f>
+        <v>0.34285714285714286</v>
       </c>
       <c r="D6" s="34" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="34"/>
       <c r="F6" s="37">
-        <f>(F20-E9)+1</f>
-        <v>25</v>
+        <f>(F31-E9)+1</f>
+        <v>54</v>
       </c>
       <c r="G6" s="37"/>
     </row>
@@ -4226,7 +4304,7 @@
         <v>44652</v>
       </c>
       <c r="G11" s="10">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H11" s="19"/>
       <c r="I11" s="19"/>
@@ -4709,7 +4787,7 @@
         <v>44663</v>
       </c>
       <c r="G14" s="10">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H14" s="19"/>
       <c r="I14" s="19"/>
@@ -5031,7 +5109,7 @@
         <v>44664</v>
       </c>
       <c r="G16" s="10">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="19"/>
@@ -5671,10 +5749,11 @@
         <v>44669</v>
       </c>
       <c r="F20" s="13">
-        <v>44669</v>
+        <f>WORKDAY(E20,(D20-1))</f>
+        <v>44670</v>
       </c>
       <c r="G20" s="10">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H20" s="19"/>
       <c r="I20" s="19"/>
@@ -5817,26 +5896,1785 @@
       <c r="EP20" s="19"/>
       <c r="EQ20" s="19"/>
     </row>
-    <row r="23" spans="2:147" x14ac:dyDescent="0.3">
-      <c r="C23" s="1"/>
+    <row r="21" spans="2:147" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="7">
+        <v>13</v>
+      </c>
+      <c r="C21" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="26">
+        <v>1</v>
+      </c>
+      <c r="E21" s="9">
+        <v>44687</v>
+      </c>
+      <c r="F21" s="13">
+        <f>WORKDAY(E21,(D21-1))</f>
+        <v>44687</v>
+      </c>
+      <c r="G21" s="10">
+        <v>0</v>
+      </c>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="19"/>
+      <c r="Q21" s="19"/>
+      <c r="R21" s="19"/>
+      <c r="S21" s="19"/>
+      <c r="T21" s="19"/>
+      <c r="U21" s="19"/>
+      <c r="V21" s="19"/>
+      <c r="W21" s="19"/>
+      <c r="X21" s="19"/>
+      <c r="Y21" s="19"/>
+      <c r="Z21" s="19"/>
+      <c r="AA21" s="19"/>
+      <c r="AB21" s="19"/>
+      <c r="AC21" s="19"/>
+      <c r="AD21" s="19"/>
+      <c r="AE21" s="19"/>
+      <c r="AF21" s="19"/>
+      <c r="AG21" s="19"/>
+      <c r="AH21" s="19"/>
+      <c r="AI21" s="19"/>
+      <c r="AJ21" s="19"/>
+      <c r="AK21" s="19"/>
+      <c r="AL21" s="19"/>
+      <c r="AM21" s="19"/>
+      <c r="AN21" s="19"/>
+      <c r="AO21" s="19"/>
+      <c r="AP21" s="19"/>
+      <c r="AQ21" s="19"/>
+      <c r="AR21" s="19"/>
+      <c r="AS21" s="19"/>
+      <c r="AT21" s="19"/>
+      <c r="AU21" s="19"/>
+      <c r="AV21" s="19"/>
+      <c r="AW21" s="19"/>
+      <c r="AX21" s="19"/>
+      <c r="AY21" s="19"/>
+      <c r="AZ21" s="19"/>
+      <c r="BA21" s="19"/>
+      <c r="BB21" s="19"/>
+      <c r="BC21" s="19"/>
+      <c r="BD21" s="19"/>
+      <c r="BE21" s="19"/>
+      <c r="BF21" s="19"/>
+      <c r="BG21" s="19"/>
+      <c r="BH21" s="19"/>
+      <c r="BI21" s="19"/>
+      <c r="BJ21" s="19"/>
+      <c r="BK21" s="19"/>
+      <c r="BL21" s="19"/>
+      <c r="BM21" s="19"/>
+      <c r="BN21" s="19"/>
+      <c r="BO21" s="19"/>
+      <c r="BP21" s="19"/>
+      <c r="BQ21" s="19"/>
+      <c r="BR21" s="19"/>
+      <c r="BS21" s="19"/>
+      <c r="BT21" s="19"/>
+      <c r="BU21" s="19"/>
+      <c r="BV21" s="19"/>
+      <c r="BW21" s="19"/>
+      <c r="BX21" s="19"/>
+      <c r="BY21" s="19"/>
+      <c r="BZ21" s="19"/>
+      <c r="CA21" s="19"/>
+      <c r="CB21" s="19"/>
+      <c r="CC21" s="19"/>
+      <c r="CD21" s="19"/>
+      <c r="CE21" s="19"/>
+      <c r="CF21" s="19"/>
+      <c r="CG21" s="19"/>
+      <c r="CH21" s="19"/>
+      <c r="CI21" s="19"/>
+      <c r="CJ21" s="19"/>
+      <c r="CK21" s="19"/>
+      <c r="CL21" s="19"/>
+      <c r="CM21" s="19"/>
+      <c r="CN21" s="19"/>
+      <c r="CO21" s="19"/>
+      <c r="CP21" s="19"/>
+      <c r="CQ21" s="19"/>
+      <c r="CR21" s="19"/>
+      <c r="CS21" s="19"/>
+      <c r="CT21" s="19"/>
+      <c r="CU21" s="19"/>
+      <c r="CV21" s="19"/>
+      <c r="CW21" s="19"/>
+      <c r="CX21" s="19"/>
+      <c r="CY21" s="19"/>
+      <c r="CZ21" s="19"/>
+      <c r="DA21" s="19"/>
+      <c r="DB21" s="19"/>
+      <c r="DC21" s="19"/>
+      <c r="DD21" s="19"/>
+      <c r="DE21" s="19"/>
+      <c r="DF21" s="19"/>
+      <c r="DG21" s="19"/>
+      <c r="DH21" s="19"/>
+      <c r="DI21" s="19"/>
+      <c r="DJ21" s="19"/>
+      <c r="DK21" s="19"/>
+      <c r="DL21" s="19"/>
+      <c r="DM21" s="19"/>
+      <c r="DN21" s="19"/>
+      <c r="DO21" s="19"/>
+      <c r="DP21" s="19"/>
+      <c r="DQ21" s="19"/>
+      <c r="DR21" s="19"/>
+      <c r="DS21" s="19"/>
+      <c r="DT21" s="19"/>
+      <c r="DU21" s="19"/>
+      <c r="DV21" s="19"/>
+      <c r="DW21" s="19"/>
+      <c r="DX21" s="19"/>
+      <c r="DY21" s="19"/>
+      <c r="DZ21" s="19"/>
+      <c r="EA21" s="19"/>
+      <c r="EB21" s="19"/>
+      <c r="EC21" s="19"/>
+      <c r="ED21" s="19"/>
+      <c r="EE21" s="19"/>
+      <c r="EF21" s="19"/>
+      <c r="EG21" s="19"/>
+      <c r="EH21" s="19"/>
+      <c r="EI21" s="19"/>
+      <c r="EJ21" s="19"/>
+      <c r="EK21" s="19"/>
+      <c r="EL21" s="19"/>
+      <c r="EM21" s="19"/>
+      <c r="EN21" s="19"/>
+      <c r="EO21" s="19"/>
+      <c r="EP21" s="19"/>
+      <c r="EQ21" s="19"/>
     </row>
-    <row r="24" spans="2:147" x14ac:dyDescent="0.3">
-      <c r="C24" s="1"/>
+    <row r="22" spans="2:147" s="2" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="7">
+        <v>14</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="26">
+        <v>1</v>
+      </c>
+      <c r="E22" s="9">
+        <v>44688</v>
+      </c>
+      <c r="F22" s="13">
+        <f>WORKDAY(E22,(D22-1))</f>
+        <v>44688</v>
+      </c>
+      <c r="G22" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="19"/>
+      <c r="Q22" s="19"/>
+      <c r="R22" s="19"/>
+      <c r="S22" s="19"/>
+      <c r="T22" s="19"/>
+      <c r="U22" s="19"/>
+      <c r="V22" s="19"/>
+      <c r="W22" s="19"/>
+      <c r="X22" s="19"/>
+      <c r="Y22" s="19"/>
+      <c r="Z22" s="19"/>
+      <c r="AA22" s="19"/>
+      <c r="AB22" s="19"/>
+      <c r="AC22" s="19"/>
+      <c r="AD22" s="19"/>
+      <c r="AE22" s="19"/>
+      <c r="AF22" s="19"/>
+      <c r="AG22" s="19"/>
+      <c r="AH22" s="19"/>
+      <c r="AI22" s="19"/>
+      <c r="AJ22" s="19"/>
+      <c r="AK22" s="19"/>
+      <c r="AL22" s="19"/>
+      <c r="AM22" s="19"/>
+      <c r="AN22" s="19"/>
+      <c r="AO22" s="19"/>
+      <c r="AP22" s="19"/>
+      <c r="AQ22" s="19"/>
+      <c r="AR22" s="19"/>
+      <c r="AS22" s="19"/>
+      <c r="AT22" s="19"/>
+      <c r="AU22" s="19"/>
+      <c r="AV22" s="19"/>
+      <c r="AW22" s="19"/>
+      <c r="AX22" s="19"/>
+      <c r="AY22" s="19"/>
+      <c r="AZ22" s="19"/>
+      <c r="BA22" s="19"/>
+      <c r="BB22" s="19"/>
+      <c r="BC22" s="19"/>
+      <c r="BD22" s="19"/>
+      <c r="BE22" s="19"/>
+      <c r="BF22" s="19"/>
+      <c r="BG22" s="19"/>
+      <c r="BH22" s="19"/>
+      <c r="BI22" s="19"/>
+      <c r="BJ22" s="19"/>
+      <c r="BK22" s="19"/>
+      <c r="BL22" s="19"/>
+      <c r="BM22" s="19"/>
+      <c r="BN22" s="19"/>
+      <c r="BO22" s="19"/>
+      <c r="BP22" s="19"/>
+      <c r="BQ22" s="19"/>
+      <c r="BR22" s="19"/>
+      <c r="BS22" s="19"/>
+      <c r="BT22" s="19"/>
+      <c r="BU22" s="19"/>
+      <c r="BV22" s="19"/>
+      <c r="BW22" s="19"/>
+      <c r="BX22" s="19"/>
+      <c r="BY22" s="19"/>
+      <c r="BZ22" s="19"/>
+      <c r="CA22" s="19"/>
+      <c r="CB22" s="19"/>
+      <c r="CC22" s="19"/>
+      <c r="CD22" s="19"/>
+      <c r="CE22" s="19"/>
+      <c r="CF22" s="19"/>
+      <c r="CG22" s="19"/>
+      <c r="CH22" s="19"/>
+      <c r="CI22" s="19"/>
+      <c r="CJ22" s="19"/>
+      <c r="CK22" s="19"/>
+      <c r="CL22" s="19"/>
+      <c r="CM22" s="19"/>
+      <c r="CN22" s="19"/>
+      <c r="CO22" s="19"/>
+      <c r="CP22" s="19"/>
+      <c r="CQ22" s="19"/>
+      <c r="CR22" s="19"/>
+      <c r="CS22" s="19"/>
+      <c r="CT22" s="19"/>
+      <c r="CU22" s="19"/>
+      <c r="CV22" s="19"/>
+      <c r="CW22" s="19"/>
+      <c r="CX22" s="19"/>
+      <c r="CY22" s="19"/>
+      <c r="CZ22" s="19"/>
+      <c r="DA22" s="19"/>
+      <c r="DB22" s="19"/>
+      <c r="DC22" s="19"/>
+      <c r="DD22" s="19"/>
+      <c r="DE22" s="19"/>
+      <c r="DF22" s="19"/>
+      <c r="DG22" s="19"/>
+      <c r="DH22" s="19"/>
+      <c r="DI22" s="19"/>
+      <c r="DJ22" s="19"/>
+      <c r="DK22" s="19"/>
+      <c r="DL22" s="19"/>
+      <c r="DM22" s="19"/>
+      <c r="DN22" s="19"/>
+      <c r="DO22" s="19"/>
+      <c r="DP22" s="19"/>
+      <c r="DQ22" s="19"/>
+      <c r="DR22" s="19"/>
+      <c r="DS22" s="19"/>
+      <c r="DT22" s="19"/>
+      <c r="DU22" s="19"/>
+      <c r="DV22" s="19"/>
+      <c r="DW22" s="19"/>
+      <c r="DX22" s="19"/>
+      <c r="DY22" s="19"/>
+      <c r="DZ22" s="19"/>
+      <c r="EA22" s="19"/>
+      <c r="EB22" s="19"/>
+      <c r="EC22" s="19"/>
+      <c r="ED22" s="19"/>
+      <c r="EE22" s="19"/>
+      <c r="EF22" s="19"/>
+      <c r="EG22" s="19"/>
+      <c r="EH22" s="19"/>
+      <c r="EI22" s="19"/>
+      <c r="EJ22" s="19"/>
+      <c r="EK22" s="19"/>
+      <c r="EL22" s="19"/>
+      <c r="EM22" s="19"/>
+      <c r="EN22" s="19"/>
+      <c r="EO22" s="19"/>
+      <c r="EP22" s="19"/>
+      <c r="EQ22" s="19"/>
+    </row>
+    <row r="23" spans="2:147" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="7">
+        <v>15</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="26">
+        <v>1</v>
+      </c>
+      <c r="E23" s="9">
+        <v>44688</v>
+      </c>
+      <c r="F23" s="13">
+        <f>WORKDAY(E23,(D23-1))</f>
+        <v>44688</v>
+      </c>
+      <c r="G23" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="19"/>
+      <c r="O23" s="19"/>
+      <c r="P23" s="19"/>
+      <c r="Q23" s="19"/>
+      <c r="R23" s="19"/>
+      <c r="S23" s="19"/>
+      <c r="T23" s="19"/>
+      <c r="U23" s="19"/>
+      <c r="V23" s="19"/>
+      <c r="W23" s="19"/>
+      <c r="X23" s="19"/>
+      <c r="Y23" s="19"/>
+      <c r="Z23" s="19"/>
+      <c r="AA23" s="19"/>
+      <c r="AB23" s="19"/>
+      <c r="AC23" s="19"/>
+      <c r="AD23" s="19"/>
+      <c r="AE23" s="19"/>
+      <c r="AF23" s="19"/>
+      <c r="AG23" s="19"/>
+      <c r="AH23" s="19"/>
+      <c r="AI23" s="19"/>
+      <c r="AJ23" s="19"/>
+      <c r="AK23" s="19"/>
+      <c r="AL23" s="19"/>
+      <c r="AM23" s="19"/>
+      <c r="AN23" s="19"/>
+      <c r="AO23" s="19"/>
+      <c r="AP23" s="19"/>
+      <c r="AQ23" s="19"/>
+      <c r="AR23" s="19"/>
+      <c r="AS23" s="19"/>
+      <c r="AT23" s="19"/>
+      <c r="AU23" s="19"/>
+      <c r="AV23" s="19"/>
+      <c r="AW23" s="19"/>
+      <c r="AX23" s="19"/>
+      <c r="AY23" s="19"/>
+      <c r="AZ23" s="19"/>
+      <c r="BA23" s="19"/>
+      <c r="BB23" s="19"/>
+      <c r="BC23" s="19"/>
+      <c r="BD23" s="19"/>
+      <c r="BE23" s="19"/>
+      <c r="BF23" s="19"/>
+      <c r="BG23" s="19"/>
+      <c r="BH23" s="19"/>
+      <c r="BI23" s="19"/>
+      <c r="BJ23" s="19"/>
+      <c r="BK23" s="19"/>
+      <c r="BL23" s="19"/>
+      <c r="BM23" s="19"/>
+      <c r="BN23" s="19"/>
+      <c r="BO23" s="19"/>
+      <c r="BP23" s="19"/>
+      <c r="BQ23" s="19"/>
+      <c r="BR23" s="19"/>
+      <c r="BS23" s="19"/>
+      <c r="BT23" s="19"/>
+      <c r="BU23" s="19"/>
+      <c r="BV23" s="19"/>
+      <c r="BW23" s="19"/>
+      <c r="BX23" s="19"/>
+      <c r="BY23" s="19"/>
+      <c r="BZ23" s="19"/>
+      <c r="CA23" s="19"/>
+      <c r="CB23" s="19"/>
+      <c r="CC23" s="19"/>
+      <c r="CD23" s="19"/>
+      <c r="CE23" s="19"/>
+      <c r="CF23" s="19"/>
+      <c r="CG23" s="19"/>
+      <c r="CH23" s="19"/>
+      <c r="CI23" s="19"/>
+      <c r="CJ23" s="19"/>
+      <c r="CK23" s="19"/>
+      <c r="CL23" s="19"/>
+      <c r="CM23" s="19"/>
+      <c r="CN23" s="19"/>
+      <c r="CO23" s="19"/>
+      <c r="CP23" s="19"/>
+      <c r="CQ23" s="19"/>
+      <c r="CR23" s="19"/>
+      <c r="CS23" s="19"/>
+      <c r="CT23" s="19"/>
+      <c r="CU23" s="19"/>
+      <c r="CV23" s="19"/>
+      <c r="CW23" s="19"/>
+      <c r="CX23" s="19"/>
+      <c r="CY23" s="19"/>
+      <c r="CZ23" s="19"/>
+      <c r="DA23" s="19"/>
+      <c r="DB23" s="19"/>
+      <c r="DC23" s="19"/>
+      <c r="DD23" s="19"/>
+      <c r="DE23" s="19"/>
+      <c r="DF23" s="19"/>
+      <c r="DG23" s="19"/>
+      <c r="DH23" s="19"/>
+      <c r="DI23" s="19"/>
+      <c r="DJ23" s="19"/>
+      <c r="DK23" s="19"/>
+      <c r="DL23" s="19"/>
+      <c r="DM23" s="19"/>
+      <c r="DN23" s="19"/>
+      <c r="DO23" s="19"/>
+      <c r="DP23" s="19"/>
+      <c r="DQ23" s="19"/>
+      <c r="DR23" s="19"/>
+      <c r="DS23" s="19"/>
+      <c r="DT23" s="19"/>
+      <c r="DU23" s="19"/>
+      <c r="DV23" s="19"/>
+      <c r="DW23" s="19"/>
+      <c r="DX23" s="19"/>
+      <c r="DY23" s="19"/>
+      <c r="DZ23" s="19"/>
+      <c r="EA23" s="19"/>
+      <c r="EB23" s="19"/>
+      <c r="EC23" s="19"/>
+      <c r="ED23" s="19"/>
+      <c r="EE23" s="19"/>
+      <c r="EF23" s="19"/>
+      <c r="EG23" s="19"/>
+      <c r="EH23" s="19"/>
+      <c r="EI23" s="19"/>
+      <c r="EJ23" s="19"/>
+      <c r="EK23" s="19"/>
+      <c r="EL23" s="19"/>
+      <c r="EM23" s="19"/>
+      <c r="EN23" s="19"/>
+      <c r="EO23" s="19"/>
+      <c r="EP23" s="19"/>
+      <c r="EQ23" s="19"/>
+    </row>
+    <row r="24" spans="2:147" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="7">
+        <v>16</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="26">
+        <v>1</v>
+      </c>
+      <c r="E24" s="9">
+        <v>44689</v>
+      </c>
+      <c r="F24" s="13">
+        <f>WORKDAY(E24,(D24-1))</f>
+        <v>44689</v>
+      </c>
+      <c r="G24" s="10">
+        <v>0</v>
+      </c>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19"/>
+      <c r="O24" s="19"/>
+      <c r="P24" s="19"/>
+      <c r="Q24" s="19"/>
+      <c r="R24" s="19"/>
+      <c r="S24" s="19"/>
+      <c r="T24" s="19"/>
+      <c r="U24" s="19"/>
+      <c r="V24" s="19"/>
+      <c r="W24" s="19"/>
+      <c r="X24" s="19"/>
+      <c r="Y24" s="19"/>
+      <c r="Z24" s="19"/>
+      <c r="AA24" s="19"/>
+      <c r="AB24" s="19"/>
+      <c r="AC24" s="19"/>
+      <c r="AD24" s="19"/>
+      <c r="AE24" s="19"/>
+      <c r="AF24" s="19"/>
+      <c r="AG24" s="19"/>
+      <c r="AH24" s="19"/>
+      <c r="AI24" s="19"/>
+      <c r="AJ24" s="19"/>
+      <c r="AK24" s="19"/>
+      <c r="AL24" s="19"/>
+      <c r="AM24" s="19"/>
+      <c r="AN24" s="19"/>
+      <c r="AO24" s="19"/>
+      <c r="AP24" s="19"/>
+      <c r="AQ24" s="19"/>
+      <c r="AR24" s="19"/>
+      <c r="AS24" s="19"/>
+      <c r="AT24" s="19"/>
+      <c r="AU24" s="19"/>
+      <c r="AV24" s="19"/>
+      <c r="AW24" s="19"/>
+      <c r="AX24" s="19"/>
+      <c r="AY24" s="19"/>
+      <c r="AZ24" s="19"/>
+      <c r="BA24" s="19"/>
+      <c r="BB24" s="19"/>
+      <c r="BC24" s="19"/>
+      <c r="BD24" s="19"/>
+      <c r="BE24" s="19"/>
+      <c r="BF24" s="19"/>
+      <c r="BG24" s="19"/>
+      <c r="BH24" s="19"/>
+      <c r="BI24" s="19"/>
+      <c r="BJ24" s="19"/>
+      <c r="BK24" s="19"/>
+      <c r="BL24" s="19"/>
+      <c r="BM24" s="19"/>
+      <c r="BN24" s="19"/>
+      <c r="BO24" s="19"/>
+      <c r="BP24" s="19"/>
+      <c r="BQ24" s="19"/>
+      <c r="BR24" s="19"/>
+      <c r="BS24" s="19"/>
+      <c r="BT24" s="19"/>
+      <c r="BU24" s="19"/>
+      <c r="BV24" s="19"/>
+      <c r="BW24" s="19"/>
+      <c r="BX24" s="19"/>
+      <c r="BY24" s="19"/>
+      <c r="BZ24" s="19"/>
+      <c r="CA24" s="19"/>
+      <c r="CB24" s="19"/>
+      <c r="CC24" s="19"/>
+      <c r="CD24" s="19"/>
+      <c r="CE24" s="19"/>
+      <c r="CF24" s="19"/>
+      <c r="CG24" s="19"/>
+      <c r="CH24" s="19"/>
+      <c r="CI24" s="19"/>
+      <c r="CJ24" s="19"/>
+      <c r="CK24" s="19"/>
+      <c r="CL24" s="19"/>
+      <c r="CM24" s="19"/>
+      <c r="CN24" s="19"/>
+      <c r="CO24" s="19"/>
+      <c r="CP24" s="19"/>
+      <c r="CQ24" s="19"/>
+      <c r="CR24" s="19"/>
+      <c r="CS24" s="19"/>
+      <c r="CT24" s="19"/>
+      <c r="CU24" s="19"/>
+      <c r="CV24" s="19"/>
+      <c r="CW24" s="19"/>
+      <c r="CX24" s="19"/>
+      <c r="CY24" s="19"/>
+      <c r="CZ24" s="19"/>
+      <c r="DA24" s="19"/>
+      <c r="DB24" s="19"/>
+      <c r="DC24" s="19"/>
+      <c r="DD24" s="19"/>
+      <c r="DE24" s="19"/>
+      <c r="DF24" s="19"/>
+      <c r="DG24" s="19"/>
+      <c r="DH24" s="19"/>
+      <c r="DI24" s="19"/>
+      <c r="DJ24" s="19"/>
+      <c r="DK24" s="19"/>
+      <c r="DL24" s="19"/>
+      <c r="DM24" s="19"/>
+      <c r="DN24" s="19"/>
+      <c r="DO24" s="19"/>
+      <c r="DP24" s="19"/>
+      <c r="DQ24" s="19"/>
+      <c r="DR24" s="19"/>
+      <c r="DS24" s="19"/>
+      <c r="DT24" s="19"/>
+      <c r="DU24" s="19"/>
+      <c r="DV24" s="19"/>
+      <c r="DW24" s="19"/>
+      <c r="DX24" s="19"/>
+      <c r="DY24" s="19"/>
+      <c r="DZ24" s="19"/>
+      <c r="EA24" s="19"/>
+      <c r="EB24" s="19"/>
+      <c r="EC24" s="19"/>
+      <c r="ED24" s="19"/>
+      <c r="EE24" s="19"/>
+      <c r="EF24" s="19"/>
+      <c r="EG24" s="19"/>
+      <c r="EH24" s="19"/>
+      <c r="EI24" s="19"/>
+      <c r="EJ24" s="19"/>
+      <c r="EK24" s="19"/>
+      <c r="EL24" s="19"/>
+      <c r="EM24" s="19"/>
+      <c r="EN24" s="19"/>
+      <c r="EO24" s="19"/>
+      <c r="EP24" s="19"/>
+      <c r="EQ24" s="19"/>
+    </row>
+    <row r="25" spans="2:147" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="7">
+        <v>17</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="26">
+        <v>1</v>
+      </c>
+      <c r="E25" s="9">
+        <v>44690</v>
+      </c>
+      <c r="F25" s="13">
+        <f>WORKDAY(E25,(D25-1))</f>
+        <v>44690</v>
+      </c>
+      <c r="G25" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="19"/>
+      <c r="P25" s="19"/>
+      <c r="Q25" s="19"/>
+      <c r="R25" s="19"/>
+      <c r="S25" s="19"/>
+      <c r="T25" s="19"/>
+      <c r="U25" s="19"/>
+      <c r="V25" s="19"/>
+      <c r="W25" s="19"/>
+      <c r="X25" s="19"/>
+      <c r="Y25" s="19"/>
+      <c r="Z25" s="19"/>
+      <c r="AA25" s="19"/>
+      <c r="AB25" s="19"/>
+      <c r="AC25" s="19"/>
+      <c r="AD25" s="19"/>
+      <c r="AE25" s="19"/>
+      <c r="AF25" s="19"/>
+      <c r="AG25" s="19"/>
+      <c r="AH25" s="19"/>
+      <c r="AI25" s="19"/>
+      <c r="AJ25" s="19"/>
+      <c r="AK25" s="19"/>
+      <c r="AL25" s="19"/>
+      <c r="AM25" s="19"/>
+      <c r="AN25" s="19"/>
+      <c r="AO25" s="19"/>
+      <c r="AP25" s="19"/>
+      <c r="AQ25" s="19"/>
+      <c r="AR25" s="19"/>
+      <c r="AS25" s="19"/>
+      <c r="AT25" s="19"/>
+      <c r="AU25" s="19"/>
+      <c r="AV25" s="19"/>
+      <c r="AW25" s="19"/>
+      <c r="AX25" s="19"/>
+      <c r="AY25" s="19"/>
+      <c r="AZ25" s="19"/>
+      <c r="BA25" s="19"/>
+      <c r="BB25" s="19"/>
+      <c r="BC25" s="19"/>
+      <c r="BD25" s="19"/>
+      <c r="BE25" s="19"/>
+      <c r="BF25" s="19"/>
+      <c r="BG25" s="19"/>
+      <c r="BH25" s="19"/>
+      <c r="BI25" s="19"/>
+      <c r="BJ25" s="19"/>
+      <c r="BK25" s="19"/>
+      <c r="BL25" s="19"/>
+      <c r="BM25" s="19"/>
+      <c r="BN25" s="19"/>
+      <c r="BO25" s="19"/>
+      <c r="BP25" s="19"/>
+      <c r="BQ25" s="19"/>
+      <c r="BR25" s="19"/>
+      <c r="BS25" s="19"/>
+      <c r="BT25" s="19"/>
+      <c r="BU25" s="19"/>
+      <c r="BV25" s="19"/>
+      <c r="BW25" s="19"/>
+      <c r="BX25" s="19"/>
+      <c r="BY25" s="19"/>
+      <c r="BZ25" s="19"/>
+      <c r="CA25" s="19"/>
+      <c r="CB25" s="19"/>
+      <c r="CC25" s="19"/>
+      <c r="CD25" s="19"/>
+      <c r="CE25" s="19"/>
+      <c r="CF25" s="19"/>
+      <c r="CG25" s="19"/>
+      <c r="CH25" s="19"/>
+      <c r="CI25" s="19"/>
+      <c r="CJ25" s="19"/>
+      <c r="CK25" s="19"/>
+      <c r="CL25" s="19"/>
+      <c r="CM25" s="19"/>
+      <c r="CN25" s="19"/>
+      <c r="CO25" s="19"/>
+      <c r="CP25" s="19"/>
+      <c r="CQ25" s="19"/>
+      <c r="CR25" s="19"/>
+      <c r="CS25" s="19"/>
+      <c r="CT25" s="19"/>
+      <c r="CU25" s="19"/>
+      <c r="CV25" s="19"/>
+      <c r="CW25" s="19"/>
+      <c r="CX25" s="19"/>
+      <c r="CY25" s="19"/>
+      <c r="CZ25" s="19"/>
+      <c r="DA25" s="19"/>
+      <c r="DB25" s="19"/>
+      <c r="DC25" s="19"/>
+      <c r="DD25" s="19"/>
+      <c r="DE25" s="19"/>
+      <c r="DF25" s="19"/>
+      <c r="DG25" s="19"/>
+      <c r="DH25" s="19"/>
+      <c r="DI25" s="19"/>
+      <c r="DJ25" s="19"/>
+      <c r="DK25" s="19"/>
+      <c r="DL25" s="19"/>
+      <c r="DM25" s="19"/>
+      <c r="DN25" s="19"/>
+      <c r="DO25" s="19"/>
+      <c r="DP25" s="19"/>
+      <c r="DQ25" s="19"/>
+      <c r="DR25" s="19"/>
+      <c r="DS25" s="19"/>
+      <c r="DT25" s="19"/>
+      <c r="DU25" s="19"/>
+      <c r="DV25" s="19"/>
+      <c r="DW25" s="19"/>
+      <c r="DX25" s="19"/>
+      <c r="DY25" s="19"/>
+      <c r="DZ25" s="19"/>
+      <c r="EA25" s="19"/>
+      <c r="EB25" s="19"/>
+      <c r="EC25" s="19"/>
+      <c r="ED25" s="19"/>
+      <c r="EE25" s="19"/>
+      <c r="EF25" s="19"/>
+      <c r="EG25" s="19"/>
+      <c r="EH25" s="19"/>
+      <c r="EI25" s="19"/>
+      <c r="EJ25" s="19"/>
+      <c r="EK25" s="19"/>
+      <c r="EL25" s="19"/>
+      <c r="EM25" s="19"/>
+      <c r="EN25" s="19"/>
+      <c r="EO25" s="19"/>
+      <c r="EP25" s="19"/>
+      <c r="EQ25" s="19"/>
+    </row>
+    <row r="26" spans="2:147" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="7">
+        <v>18</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="26">
+        <v>1</v>
+      </c>
+      <c r="E26" s="9">
+        <v>44692</v>
+      </c>
+      <c r="F26" s="13">
+        <f>WORKDAY(E26,(D26-1))</f>
+        <v>44692</v>
+      </c>
+      <c r="G26" s="10">
+        <v>0</v>
+      </c>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="19"/>
+      <c r="P26" s="19"/>
+      <c r="Q26" s="19"/>
+      <c r="R26" s="19"/>
+      <c r="S26" s="19"/>
+      <c r="T26" s="19"/>
+      <c r="U26" s="19"/>
+      <c r="V26" s="19"/>
+      <c r="W26" s="19"/>
+      <c r="X26" s="19"/>
+      <c r="Y26" s="19"/>
+      <c r="Z26" s="19"/>
+      <c r="AA26" s="19"/>
+      <c r="AB26" s="19"/>
+      <c r="AC26" s="19"/>
+      <c r="AD26" s="19"/>
+      <c r="AE26" s="19"/>
+      <c r="AF26" s="19"/>
+      <c r="AG26" s="19"/>
+      <c r="AH26" s="19"/>
+      <c r="AI26" s="19"/>
+      <c r="AJ26" s="19"/>
+      <c r="AK26" s="19"/>
+      <c r="AL26" s="19"/>
+      <c r="AM26" s="19"/>
+      <c r="AN26" s="19"/>
+      <c r="AO26" s="19"/>
+      <c r="AP26" s="19"/>
+      <c r="AQ26" s="19"/>
+      <c r="AR26" s="19"/>
+      <c r="AS26" s="19"/>
+      <c r="AT26" s="19"/>
+      <c r="AU26" s="19"/>
+      <c r="AV26" s="19"/>
+      <c r="AW26" s="19"/>
+      <c r="AX26" s="19"/>
+      <c r="AY26" s="19"/>
+      <c r="AZ26" s="19"/>
+      <c r="BA26" s="19"/>
+      <c r="BB26" s="19"/>
+      <c r="BC26" s="19"/>
+      <c r="BD26" s="19"/>
+      <c r="BE26" s="19"/>
+      <c r="BF26" s="19"/>
+      <c r="BG26" s="19"/>
+      <c r="BH26" s="19"/>
+      <c r="BI26" s="19"/>
+      <c r="BJ26" s="19"/>
+      <c r="BK26" s="19"/>
+      <c r="BL26" s="19"/>
+      <c r="BM26" s="19"/>
+      <c r="BN26" s="19"/>
+      <c r="BO26" s="19"/>
+      <c r="BP26" s="19"/>
+      <c r="BQ26" s="19"/>
+      <c r="BR26" s="19"/>
+      <c r="BS26" s="19"/>
+      <c r="BT26" s="19"/>
+      <c r="BU26" s="19"/>
+      <c r="BV26" s="19"/>
+      <c r="BW26" s="19"/>
+      <c r="BX26" s="19"/>
+      <c r="BY26" s="19"/>
+      <c r="BZ26" s="19"/>
+      <c r="CA26" s="19"/>
+      <c r="CB26" s="19"/>
+      <c r="CC26" s="19"/>
+      <c r="CD26" s="19"/>
+      <c r="CE26" s="19"/>
+      <c r="CF26" s="19"/>
+      <c r="CG26" s="19"/>
+      <c r="CH26" s="19"/>
+      <c r="CI26" s="19"/>
+      <c r="CJ26" s="19"/>
+      <c r="CK26" s="19"/>
+      <c r="CL26" s="19"/>
+      <c r="CM26" s="19"/>
+      <c r="CN26" s="19"/>
+      <c r="CO26" s="19"/>
+      <c r="CP26" s="19"/>
+      <c r="CQ26" s="19"/>
+      <c r="CR26" s="19"/>
+      <c r="CS26" s="19"/>
+      <c r="CT26" s="19"/>
+      <c r="CU26" s="19"/>
+      <c r="CV26" s="19"/>
+      <c r="CW26" s="19"/>
+      <c r="CX26" s="19"/>
+      <c r="CY26" s="19"/>
+      <c r="CZ26" s="19"/>
+      <c r="DA26" s="19"/>
+      <c r="DB26" s="19"/>
+      <c r="DC26" s="19"/>
+      <c r="DD26" s="19"/>
+      <c r="DE26" s="19"/>
+      <c r="DF26" s="19"/>
+      <c r="DG26" s="19"/>
+      <c r="DH26" s="19"/>
+      <c r="DI26" s="19"/>
+      <c r="DJ26" s="19"/>
+      <c r="DK26" s="19"/>
+      <c r="DL26" s="19"/>
+      <c r="DM26" s="19"/>
+      <c r="DN26" s="19"/>
+      <c r="DO26" s="19"/>
+      <c r="DP26" s="19"/>
+      <c r="DQ26" s="19"/>
+      <c r="DR26" s="19"/>
+      <c r="DS26" s="19"/>
+      <c r="DT26" s="19"/>
+      <c r="DU26" s="19"/>
+      <c r="DV26" s="19"/>
+      <c r="DW26" s="19"/>
+      <c r="DX26" s="19"/>
+      <c r="DY26" s="19"/>
+      <c r="DZ26" s="19"/>
+      <c r="EA26" s="19"/>
+      <c r="EB26" s="19"/>
+      <c r="EC26" s="19"/>
+      <c r="ED26" s="19"/>
+      <c r="EE26" s="19"/>
+      <c r="EF26" s="19"/>
+      <c r="EG26" s="19"/>
+      <c r="EH26" s="19"/>
+      <c r="EI26" s="19"/>
+      <c r="EJ26" s="19"/>
+      <c r="EK26" s="19"/>
+      <c r="EL26" s="19"/>
+      <c r="EM26" s="19"/>
+      <c r="EN26" s="19"/>
+      <c r="EO26" s="19"/>
+      <c r="EP26" s="19"/>
+      <c r="EQ26" s="19"/>
+    </row>
+    <row r="27" spans="2:147" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="7">
+        <v>19</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="26">
+        <v>1</v>
+      </c>
+      <c r="E27" s="9">
+        <v>44693</v>
+      </c>
+      <c r="F27" s="13">
+        <f>WORKDAY(E27,(D27-1))</f>
+        <v>44693</v>
+      </c>
+      <c r="G27" s="10">
+        <v>0</v>
+      </c>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="19"/>
+      <c r="P27" s="19"/>
+      <c r="Q27" s="19"/>
+      <c r="R27" s="19"/>
+      <c r="S27" s="19"/>
+      <c r="T27" s="19"/>
+      <c r="U27" s="19"/>
+      <c r="V27" s="19"/>
+      <c r="W27" s="19"/>
+      <c r="X27" s="19"/>
+      <c r="Y27" s="19"/>
+      <c r="Z27" s="19"/>
+      <c r="AA27" s="19"/>
+      <c r="AB27" s="19"/>
+      <c r="AC27" s="19"/>
+      <c r="AD27" s="19"/>
+      <c r="AE27" s="19"/>
+      <c r="AF27" s="19"/>
+      <c r="AG27" s="19"/>
+      <c r="AH27" s="19"/>
+      <c r="AI27" s="19"/>
+      <c r="AJ27" s="19"/>
+      <c r="AK27" s="19"/>
+      <c r="AL27" s="19"/>
+      <c r="AM27" s="19"/>
+      <c r="AN27" s="19"/>
+      <c r="AO27" s="19"/>
+      <c r="AP27" s="19"/>
+      <c r="AQ27" s="19"/>
+      <c r="AR27" s="19"/>
+      <c r="AS27" s="19"/>
+      <c r="AT27" s="19"/>
+      <c r="AU27" s="19"/>
+      <c r="AV27" s="19"/>
+      <c r="AW27" s="19"/>
+      <c r="AX27" s="19"/>
+      <c r="AY27" s="19"/>
+      <c r="AZ27" s="19"/>
+      <c r="BA27" s="19"/>
+      <c r="BB27" s="19"/>
+      <c r="BC27" s="19"/>
+      <c r="BD27" s="19"/>
+      <c r="BE27" s="19"/>
+      <c r="BF27" s="19"/>
+      <c r="BG27" s="19"/>
+      <c r="BH27" s="19"/>
+      <c r="BI27" s="19"/>
+      <c r="BJ27" s="19"/>
+      <c r="BK27" s="19"/>
+      <c r="BL27" s="19"/>
+      <c r="BM27" s="19"/>
+      <c r="BN27" s="19"/>
+      <c r="BO27" s="19"/>
+      <c r="BP27" s="19"/>
+      <c r="BQ27" s="19"/>
+      <c r="BR27" s="19"/>
+      <c r="BS27" s="19"/>
+      <c r="BT27" s="19"/>
+      <c r="BU27" s="19"/>
+      <c r="BV27" s="19"/>
+      <c r="BW27" s="19"/>
+      <c r="BX27" s="19"/>
+      <c r="BY27" s="19"/>
+      <c r="BZ27" s="19"/>
+      <c r="CA27" s="19"/>
+      <c r="CB27" s="19"/>
+      <c r="CC27" s="19"/>
+      <c r="CD27" s="19"/>
+      <c r="CE27" s="19"/>
+      <c r="CF27" s="19"/>
+      <c r="CG27" s="19"/>
+      <c r="CH27" s="19"/>
+      <c r="CI27" s="19"/>
+      <c r="CJ27" s="19"/>
+      <c r="CK27" s="19"/>
+      <c r="CL27" s="19"/>
+      <c r="CM27" s="19"/>
+      <c r="CN27" s="19"/>
+      <c r="CO27" s="19"/>
+      <c r="CP27" s="19"/>
+      <c r="CQ27" s="19"/>
+      <c r="CR27" s="19"/>
+      <c r="CS27" s="19"/>
+      <c r="CT27" s="19"/>
+      <c r="CU27" s="19"/>
+      <c r="CV27" s="19"/>
+      <c r="CW27" s="19"/>
+      <c r="CX27" s="19"/>
+      <c r="CY27" s="19"/>
+      <c r="CZ27" s="19"/>
+      <c r="DA27" s="19"/>
+      <c r="DB27" s="19"/>
+      <c r="DC27" s="19"/>
+      <c r="DD27" s="19"/>
+      <c r="DE27" s="19"/>
+      <c r="DF27" s="19"/>
+      <c r="DG27" s="19"/>
+      <c r="DH27" s="19"/>
+      <c r="DI27" s="19"/>
+      <c r="DJ27" s="19"/>
+      <c r="DK27" s="19"/>
+      <c r="DL27" s="19"/>
+      <c r="DM27" s="19"/>
+      <c r="DN27" s="19"/>
+      <c r="DO27" s="19"/>
+      <c r="DP27" s="19"/>
+      <c r="DQ27" s="19"/>
+      <c r="DR27" s="19"/>
+      <c r="DS27" s="19"/>
+      <c r="DT27" s="19"/>
+      <c r="DU27" s="19"/>
+      <c r="DV27" s="19"/>
+      <c r="DW27" s="19"/>
+      <c r="DX27" s="19"/>
+      <c r="DY27" s="19"/>
+      <c r="DZ27" s="19"/>
+      <c r="EA27" s="19"/>
+      <c r="EB27" s="19"/>
+      <c r="EC27" s="19"/>
+      <c r="ED27" s="19"/>
+      <c r="EE27" s="19"/>
+      <c r="EF27" s="19"/>
+      <c r="EG27" s="19"/>
+      <c r="EH27" s="19"/>
+      <c r="EI27" s="19"/>
+      <c r="EJ27" s="19"/>
+      <c r="EK27" s="19"/>
+      <c r="EL27" s="19"/>
+      <c r="EM27" s="19"/>
+      <c r="EN27" s="19"/>
+      <c r="EO27" s="19"/>
+      <c r="EP27" s="19"/>
+      <c r="EQ27" s="19"/>
+    </row>
+    <row r="28" spans="2:147" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="7">
+        <v>20</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="26">
+        <v>2</v>
+      </c>
+      <c r="E28" s="9">
+        <v>44694</v>
+      </c>
+      <c r="F28" s="13">
+        <f>WORKDAY(E28,(D28-1))</f>
+        <v>44697</v>
+      </c>
+      <c r="G28" s="10">
+        <v>0</v>
+      </c>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="19"/>
+      <c r="P28" s="19"/>
+      <c r="Q28" s="19"/>
+      <c r="R28" s="19"/>
+      <c r="S28" s="19"/>
+      <c r="T28" s="19"/>
+      <c r="U28" s="19"/>
+      <c r="V28" s="19"/>
+      <c r="W28" s="19"/>
+      <c r="X28" s="19"/>
+      <c r="Y28" s="19"/>
+      <c r="Z28" s="19"/>
+      <c r="AA28" s="19"/>
+      <c r="AB28" s="19"/>
+      <c r="AC28" s="19"/>
+      <c r="AD28" s="19"/>
+      <c r="AE28" s="19"/>
+      <c r="AF28" s="19"/>
+      <c r="AG28" s="19"/>
+      <c r="AH28" s="19"/>
+      <c r="AI28" s="19"/>
+      <c r="AJ28" s="19"/>
+      <c r="AK28" s="19"/>
+      <c r="AL28" s="19"/>
+      <c r="AM28" s="19"/>
+      <c r="AN28" s="19"/>
+      <c r="AO28" s="19"/>
+      <c r="AP28" s="19"/>
+      <c r="AQ28" s="19"/>
+      <c r="AR28" s="19"/>
+      <c r="AS28" s="19"/>
+      <c r="AT28" s="19"/>
+      <c r="AU28" s="19"/>
+      <c r="AV28" s="19"/>
+      <c r="AW28" s="19"/>
+      <c r="AX28" s="19"/>
+      <c r="AY28" s="19"/>
+      <c r="AZ28" s="19"/>
+      <c r="BA28" s="19"/>
+      <c r="BB28" s="19"/>
+      <c r="BC28" s="19"/>
+      <c r="BD28" s="19"/>
+      <c r="BE28" s="19"/>
+      <c r="BF28" s="19"/>
+      <c r="BG28" s="19"/>
+      <c r="BH28" s="19"/>
+      <c r="BI28" s="19"/>
+      <c r="BJ28" s="19"/>
+      <c r="BK28" s="19"/>
+      <c r="BL28" s="19"/>
+      <c r="BM28" s="19"/>
+      <c r="BN28" s="19"/>
+      <c r="BO28" s="19"/>
+      <c r="BP28" s="19"/>
+      <c r="BQ28" s="19"/>
+      <c r="BR28" s="19"/>
+      <c r="BS28" s="19"/>
+      <c r="BT28" s="19"/>
+      <c r="BU28" s="19"/>
+      <c r="BV28" s="19"/>
+      <c r="BW28" s="19"/>
+      <c r="BX28" s="19"/>
+      <c r="BY28" s="19"/>
+      <c r="BZ28" s="19"/>
+      <c r="CA28" s="19"/>
+      <c r="CB28" s="19"/>
+      <c r="CC28" s="19"/>
+      <c r="CD28" s="19"/>
+      <c r="CE28" s="19"/>
+      <c r="CF28" s="19"/>
+      <c r="CG28" s="19"/>
+      <c r="CH28" s="19"/>
+      <c r="CI28" s="19"/>
+      <c r="CJ28" s="19"/>
+      <c r="CK28" s="19"/>
+      <c r="CL28" s="19"/>
+      <c r="CM28" s="19"/>
+      <c r="CN28" s="19"/>
+      <c r="CO28" s="19"/>
+      <c r="CP28" s="19"/>
+      <c r="CQ28" s="19"/>
+      <c r="CR28" s="19"/>
+      <c r="CS28" s="19"/>
+      <c r="CT28" s="19"/>
+      <c r="CU28" s="19"/>
+      <c r="CV28" s="19"/>
+      <c r="CW28" s="19"/>
+      <c r="CX28" s="19"/>
+      <c r="CY28" s="19"/>
+      <c r="CZ28" s="19"/>
+      <c r="DA28" s="19"/>
+      <c r="DB28" s="19"/>
+      <c r="DC28" s="19"/>
+      <c r="DD28" s="19"/>
+      <c r="DE28" s="19"/>
+      <c r="DF28" s="19"/>
+      <c r="DG28" s="19"/>
+      <c r="DH28" s="19"/>
+      <c r="DI28" s="19"/>
+      <c r="DJ28" s="19"/>
+      <c r="DK28" s="19"/>
+      <c r="DL28" s="19"/>
+      <c r="DM28" s="19"/>
+      <c r="DN28" s="19"/>
+      <c r="DO28" s="19"/>
+      <c r="DP28" s="19"/>
+      <c r="DQ28" s="19"/>
+      <c r="DR28" s="19"/>
+      <c r="DS28" s="19"/>
+      <c r="DT28" s="19"/>
+      <c r="DU28" s="19"/>
+      <c r="DV28" s="19"/>
+      <c r="DW28" s="19"/>
+      <c r="DX28" s="19"/>
+      <c r="DY28" s="19"/>
+      <c r="DZ28" s="19"/>
+      <c r="EA28" s="19"/>
+      <c r="EB28" s="19"/>
+      <c r="EC28" s="19"/>
+      <c r="ED28" s="19"/>
+      <c r="EE28" s="19"/>
+      <c r="EF28" s="19"/>
+      <c r="EG28" s="19"/>
+      <c r="EH28" s="19"/>
+      <c r="EI28" s="19"/>
+      <c r="EJ28" s="19"/>
+      <c r="EK28" s="19"/>
+      <c r="EL28" s="19"/>
+      <c r="EM28" s="19"/>
+      <c r="EN28" s="19"/>
+      <c r="EO28" s="19"/>
+      <c r="EP28" s="19"/>
+      <c r="EQ28" s="19"/>
+    </row>
+    <row r="29" spans="2:147" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="7">
+        <v>21</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="26">
+        <v>3</v>
+      </c>
+      <c r="E29" s="9">
+        <v>44695</v>
+      </c>
+      <c r="F29" s="13">
+        <f>WORKDAY(E29,(D29-1))</f>
+        <v>44698</v>
+      </c>
+      <c r="G29" s="10">
+        <v>0</v>
+      </c>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
+      <c r="O29" s="19"/>
+      <c r="P29" s="19"/>
+      <c r="Q29" s="19"/>
+      <c r="R29" s="19"/>
+      <c r="S29" s="19"/>
+      <c r="T29" s="19"/>
+      <c r="U29" s="19"/>
+      <c r="V29" s="19"/>
+      <c r="W29" s="19"/>
+      <c r="X29" s="19"/>
+      <c r="Y29" s="19"/>
+      <c r="Z29" s="19"/>
+      <c r="AA29" s="19"/>
+      <c r="AB29" s="19"/>
+      <c r="AC29" s="19"/>
+      <c r="AD29" s="19"/>
+      <c r="AE29" s="19"/>
+      <c r="AF29" s="19"/>
+      <c r="AG29" s="19"/>
+      <c r="AH29" s="19"/>
+      <c r="AI29" s="19"/>
+      <c r="AJ29" s="19"/>
+      <c r="AK29" s="19"/>
+      <c r="AL29" s="19"/>
+      <c r="AM29" s="19"/>
+      <c r="AN29" s="19"/>
+      <c r="AO29" s="19"/>
+      <c r="AP29" s="19"/>
+      <c r="AQ29" s="19"/>
+      <c r="AR29" s="19"/>
+      <c r="AS29" s="19"/>
+      <c r="AT29" s="19"/>
+      <c r="AU29" s="19"/>
+      <c r="AV29" s="19"/>
+      <c r="AW29" s="19"/>
+      <c r="AX29" s="19"/>
+      <c r="AY29" s="19"/>
+      <c r="AZ29" s="19"/>
+      <c r="BA29" s="19"/>
+      <c r="BB29" s="19"/>
+      <c r="BC29" s="19"/>
+      <c r="BD29" s="19"/>
+      <c r="BE29" s="19"/>
+      <c r="BF29" s="19"/>
+      <c r="BG29" s="19"/>
+      <c r="BH29" s="19"/>
+      <c r="BI29" s="19"/>
+      <c r="BJ29" s="19"/>
+      <c r="BK29" s="19"/>
+      <c r="BL29" s="19"/>
+      <c r="BM29" s="19"/>
+      <c r="BN29" s="19"/>
+      <c r="BO29" s="19"/>
+      <c r="BP29" s="19"/>
+      <c r="BQ29" s="19"/>
+      <c r="BR29" s="19"/>
+      <c r="BS29" s="19"/>
+      <c r="BT29" s="19"/>
+      <c r="BU29" s="19"/>
+      <c r="BV29" s="19"/>
+      <c r="BW29" s="19"/>
+      <c r="BX29" s="19"/>
+      <c r="BY29" s="19"/>
+      <c r="BZ29" s="19"/>
+      <c r="CA29" s="19"/>
+      <c r="CB29" s="19"/>
+      <c r="CC29" s="19"/>
+      <c r="CD29" s="19"/>
+      <c r="CE29" s="19"/>
+      <c r="CF29" s="19"/>
+      <c r="CG29" s="19"/>
+      <c r="CH29" s="19"/>
+      <c r="CI29" s="19"/>
+      <c r="CJ29" s="19"/>
+      <c r="CK29" s="19"/>
+      <c r="CL29" s="19"/>
+      <c r="CM29" s="19"/>
+      <c r="CN29" s="19"/>
+      <c r="CO29" s="19"/>
+      <c r="CP29" s="19"/>
+      <c r="CQ29" s="19"/>
+      <c r="CR29" s="19"/>
+      <c r="CS29" s="19"/>
+      <c r="CT29" s="19"/>
+      <c r="CU29" s="19"/>
+      <c r="CV29" s="19"/>
+      <c r="CW29" s="19"/>
+      <c r="CX29" s="19"/>
+      <c r="CY29" s="19"/>
+      <c r="CZ29" s="19"/>
+      <c r="DA29" s="19"/>
+      <c r="DB29" s="19"/>
+      <c r="DC29" s="19"/>
+      <c r="DD29" s="19"/>
+      <c r="DE29" s="19"/>
+      <c r="DF29" s="19"/>
+      <c r="DG29" s="19"/>
+      <c r="DH29" s="19"/>
+      <c r="DI29" s="19"/>
+      <c r="DJ29" s="19"/>
+      <c r="DK29" s="19"/>
+      <c r="DL29" s="19"/>
+      <c r="DM29" s="19"/>
+      <c r="DN29" s="19"/>
+      <c r="DO29" s="19"/>
+      <c r="DP29" s="19"/>
+      <c r="DQ29" s="19"/>
+      <c r="DR29" s="19"/>
+      <c r="DS29" s="19"/>
+      <c r="DT29" s="19"/>
+      <c r="DU29" s="19"/>
+      <c r="DV29" s="19"/>
+      <c r="DW29" s="19"/>
+      <c r="DX29" s="19"/>
+      <c r="DY29" s="19"/>
+      <c r="DZ29" s="19"/>
+      <c r="EA29" s="19"/>
+      <c r="EB29" s="19"/>
+      <c r="EC29" s="19"/>
+      <c r="ED29" s="19"/>
+      <c r="EE29" s="19"/>
+      <c r="EF29" s="19"/>
+      <c r="EG29" s="19"/>
+      <c r="EH29" s="19"/>
+      <c r="EI29" s="19"/>
+      <c r="EJ29" s="19"/>
+      <c r="EK29" s="19"/>
+      <c r="EL29" s="19"/>
+      <c r="EM29" s="19"/>
+      <c r="EN29" s="19"/>
+      <c r="EO29" s="19"/>
+      <c r="EP29" s="19"/>
+      <c r="EQ29" s="19"/>
+    </row>
+    <row r="30" spans="2:147" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="7">
+        <v>22</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="26">
+        <v>3</v>
+      </c>
+      <c r="E30" s="9">
+        <v>44696</v>
+      </c>
+      <c r="F30" s="13">
+        <f>WORKDAY(E30,(D30-1))</f>
+        <v>44698</v>
+      </c>
+      <c r="G30" s="10">
+        <v>0</v>
+      </c>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="19"/>
+      <c r="N30" s="19"/>
+      <c r="O30" s="19"/>
+      <c r="P30" s="19"/>
+      <c r="Q30" s="19"/>
+      <c r="R30" s="19"/>
+      <c r="S30" s="19"/>
+      <c r="T30" s="19"/>
+      <c r="U30" s="19"/>
+      <c r="V30" s="19"/>
+      <c r="W30" s="19"/>
+      <c r="X30" s="19"/>
+      <c r="Y30" s="19"/>
+      <c r="Z30" s="19"/>
+      <c r="AA30" s="19"/>
+      <c r="AB30" s="19"/>
+      <c r="AC30" s="19"/>
+      <c r="AD30" s="19"/>
+      <c r="AE30" s="19"/>
+      <c r="AF30" s="19"/>
+      <c r="AG30" s="19"/>
+      <c r="AH30" s="19"/>
+      <c r="AI30" s="19"/>
+      <c r="AJ30" s="19"/>
+      <c r="AK30" s="19"/>
+      <c r="AL30" s="19"/>
+      <c r="AM30" s="19"/>
+      <c r="AN30" s="19"/>
+      <c r="AO30" s="19"/>
+      <c r="AP30" s="19"/>
+      <c r="AQ30" s="19"/>
+      <c r="AR30" s="19"/>
+      <c r="AS30" s="19"/>
+      <c r="AT30" s="19"/>
+      <c r="AU30" s="19"/>
+      <c r="AV30" s="19"/>
+      <c r="AW30" s="19"/>
+      <c r="AX30" s="19"/>
+      <c r="AY30" s="19"/>
+      <c r="AZ30" s="19"/>
+      <c r="BA30" s="19"/>
+      <c r="BB30" s="19"/>
+      <c r="BC30" s="19"/>
+      <c r="BD30" s="19"/>
+      <c r="BE30" s="19"/>
+      <c r="BF30" s="19"/>
+      <c r="BG30" s="19"/>
+      <c r="BH30" s="19"/>
+      <c r="BI30" s="19"/>
+      <c r="BJ30" s="19"/>
+      <c r="BK30" s="19"/>
+      <c r="BL30" s="19"/>
+      <c r="BM30" s="19"/>
+      <c r="BN30" s="19"/>
+      <c r="BO30" s="19"/>
+      <c r="BP30" s="19"/>
+      <c r="BQ30" s="19"/>
+      <c r="BR30" s="19"/>
+      <c r="BS30" s="19"/>
+      <c r="BT30" s="19"/>
+      <c r="BU30" s="19"/>
+      <c r="BV30" s="19"/>
+      <c r="BW30" s="19"/>
+      <c r="BX30" s="19"/>
+      <c r="BY30" s="19"/>
+      <c r="BZ30" s="19"/>
+      <c r="CA30" s="19"/>
+      <c r="CB30" s="19"/>
+      <c r="CC30" s="19"/>
+      <c r="CD30" s="19"/>
+      <c r="CE30" s="19"/>
+      <c r="CF30" s="19"/>
+      <c r="CG30" s="19"/>
+      <c r="CH30" s="19"/>
+      <c r="CI30" s="19"/>
+      <c r="CJ30" s="19"/>
+      <c r="CK30" s="19"/>
+      <c r="CL30" s="19"/>
+      <c r="CM30" s="19"/>
+      <c r="CN30" s="19"/>
+      <c r="CO30" s="19"/>
+      <c r="CP30" s="19"/>
+      <c r="CQ30" s="19"/>
+      <c r="CR30" s="19"/>
+      <c r="CS30" s="19"/>
+      <c r="CT30" s="19"/>
+      <c r="CU30" s="19"/>
+      <c r="CV30" s="19"/>
+      <c r="CW30" s="19"/>
+      <c r="CX30" s="19"/>
+      <c r="CY30" s="19"/>
+      <c r="CZ30" s="19"/>
+      <c r="DA30" s="19"/>
+      <c r="DB30" s="19"/>
+      <c r="DC30" s="19"/>
+      <c r="DD30" s="19"/>
+      <c r="DE30" s="19"/>
+      <c r="DF30" s="19"/>
+      <c r="DG30" s="19"/>
+      <c r="DH30" s="19"/>
+      <c r="DI30" s="19"/>
+      <c r="DJ30" s="19"/>
+      <c r="DK30" s="19"/>
+      <c r="DL30" s="19"/>
+      <c r="DM30" s="19"/>
+      <c r="DN30" s="19"/>
+      <c r="DO30" s="19"/>
+      <c r="DP30" s="19"/>
+      <c r="DQ30" s="19"/>
+      <c r="DR30" s="19"/>
+      <c r="DS30" s="19"/>
+      <c r="DT30" s="19"/>
+      <c r="DU30" s="19"/>
+      <c r="DV30" s="19"/>
+      <c r="DW30" s="19"/>
+      <c r="DX30" s="19"/>
+      <c r="DY30" s="19"/>
+      <c r="DZ30" s="19"/>
+      <c r="EA30" s="19"/>
+      <c r="EB30" s="19"/>
+      <c r="EC30" s="19"/>
+      <c r="ED30" s="19"/>
+      <c r="EE30" s="19"/>
+      <c r="EF30" s="19"/>
+      <c r="EG30" s="19"/>
+      <c r="EH30" s="19"/>
+      <c r="EI30" s="19"/>
+      <c r="EJ30" s="19"/>
+      <c r="EK30" s="19"/>
+      <c r="EL30" s="19"/>
+      <c r="EM30" s="19"/>
+      <c r="EN30" s="19"/>
+      <c r="EO30" s="19"/>
+      <c r="EP30" s="19"/>
+      <c r="EQ30" s="19"/>
+    </row>
+    <row r="31" spans="2:147" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="7">
+        <v>23</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="26">
+        <v>1</v>
+      </c>
+      <c r="E31" s="9">
+        <v>44698</v>
+      </c>
+      <c r="F31" s="13">
+        <f>WORKDAY(E31,(D31-1))</f>
+        <v>44698</v>
+      </c>
+      <c r="G31" s="10">
+        <v>0</v>
+      </c>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
+      <c r="O31" s="19"/>
+      <c r="P31" s="19"/>
+      <c r="Q31" s="19"/>
+      <c r="R31" s="19"/>
+      <c r="S31" s="19"/>
+      <c r="T31" s="19"/>
+      <c r="U31" s="19"/>
+      <c r="V31" s="19"/>
+      <c r="W31" s="19"/>
+      <c r="X31" s="19"/>
+      <c r="Y31" s="19"/>
+      <c r="Z31" s="19"/>
+      <c r="AA31" s="19"/>
+      <c r="AB31" s="19"/>
+      <c r="AC31" s="19"/>
+      <c r="AD31" s="19"/>
+      <c r="AE31" s="19"/>
+      <c r="AF31" s="19"/>
+      <c r="AG31" s="19"/>
+      <c r="AH31" s="19"/>
+      <c r="AI31" s="19"/>
+      <c r="AJ31" s="19"/>
+      <c r="AK31" s="19"/>
+      <c r="AL31" s="19"/>
+      <c r="AM31" s="19"/>
+      <c r="AN31" s="19"/>
+      <c r="AO31" s="19"/>
+      <c r="AP31" s="19"/>
+      <c r="AQ31" s="19"/>
+      <c r="AR31" s="19"/>
+      <c r="AS31" s="19"/>
+      <c r="AT31" s="19"/>
+      <c r="AU31" s="19"/>
+      <c r="AV31" s="19"/>
+      <c r="AW31" s="19"/>
+      <c r="AX31" s="19"/>
+      <c r="AY31" s="19"/>
+      <c r="AZ31" s="19"/>
+      <c r="BA31" s="19"/>
+      <c r="BB31" s="19"/>
+      <c r="BC31" s="19"/>
+      <c r="BD31" s="19"/>
+      <c r="BE31" s="19"/>
+      <c r="BF31" s="19"/>
+      <c r="BG31" s="19"/>
+      <c r="BH31" s="19"/>
+      <c r="BI31" s="19"/>
+      <c r="BJ31" s="19"/>
+      <c r="BK31" s="19"/>
+      <c r="BL31" s="19"/>
+      <c r="BM31" s="19"/>
+      <c r="BN31" s="19"/>
+      <c r="BO31" s="19"/>
+      <c r="BP31" s="19"/>
+      <c r="BQ31" s="19"/>
+      <c r="BR31" s="19"/>
+      <c r="BS31" s="19"/>
+      <c r="BT31" s="19"/>
+      <c r="BU31" s="19"/>
+      <c r="BV31" s="19"/>
+      <c r="BW31" s="19"/>
+      <c r="BX31" s="19"/>
+      <c r="BY31" s="19"/>
+      <c r="BZ31" s="19"/>
+      <c r="CA31" s="19"/>
+      <c r="CB31" s="19"/>
+      <c r="CC31" s="19"/>
+      <c r="CD31" s="19"/>
+      <c r="CE31" s="19"/>
+      <c r="CF31" s="19"/>
+      <c r="CG31" s="19"/>
+      <c r="CH31" s="19"/>
+      <c r="CI31" s="19"/>
+      <c r="CJ31" s="19"/>
+      <c r="CK31" s="19"/>
+      <c r="CL31" s="19"/>
+      <c r="CM31" s="19"/>
+      <c r="CN31" s="19"/>
+      <c r="CO31" s="19"/>
+      <c r="CP31" s="19"/>
+      <c r="CQ31" s="19"/>
+      <c r="CR31" s="19"/>
+      <c r="CS31" s="19"/>
+      <c r="CT31" s="19"/>
+      <c r="CU31" s="19"/>
+      <c r="CV31" s="19"/>
+      <c r="CW31" s="19"/>
+      <c r="CX31" s="19"/>
+      <c r="CY31" s="19"/>
+      <c r="CZ31" s="19"/>
+      <c r="DA31" s="19"/>
+      <c r="DB31" s="19"/>
+      <c r="DC31" s="19"/>
+      <c r="DD31" s="19"/>
+      <c r="DE31" s="19"/>
+      <c r="DF31" s="19"/>
+      <c r="DG31" s="19"/>
+      <c r="DH31" s="19"/>
+      <c r="DI31" s="19"/>
+      <c r="DJ31" s="19"/>
+      <c r="DK31" s="19"/>
+      <c r="DL31" s="19"/>
+      <c r="DM31" s="19"/>
+      <c r="DN31" s="19"/>
+      <c r="DO31" s="19"/>
+      <c r="DP31" s="19"/>
+      <c r="DQ31" s="19"/>
+      <c r="DR31" s="19"/>
+      <c r="DS31" s="19"/>
+      <c r="DT31" s="19"/>
+      <c r="DU31" s="19"/>
+      <c r="DV31" s="19"/>
+      <c r="DW31" s="19"/>
+      <c r="DX31" s="19"/>
+      <c r="DY31" s="19"/>
+      <c r="DZ31" s="19"/>
+      <c r="EA31" s="19"/>
+      <c r="EB31" s="19"/>
+      <c r="EC31" s="19"/>
+      <c r="ED31" s="19"/>
+      <c r="EE31" s="19"/>
+      <c r="EF31" s="19"/>
+      <c r="EG31" s="19"/>
+      <c r="EH31" s="19"/>
+      <c r="EI31" s="19"/>
+      <c r="EJ31" s="19"/>
+      <c r="EK31" s="19"/>
+      <c r="EL31" s="19"/>
+      <c r="EM31" s="19"/>
+      <c r="EN31" s="19"/>
+      <c r="EO31" s="19"/>
+      <c r="EP31" s="19"/>
+      <c r="EQ31" s="19"/>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C34" s="1"/>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C35" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="EK7:EQ7"/>
-    <mergeCell ref="BE7:BK7"/>
-    <mergeCell ref="BS7:BY7"/>
-    <mergeCell ref="BZ7:CF7"/>
-    <mergeCell ref="CG7:CM7"/>
-    <mergeCell ref="CN7:CT7"/>
-    <mergeCell ref="CU7:DA7"/>
-    <mergeCell ref="DB7:DH7"/>
-    <mergeCell ref="DI7:DO7"/>
-    <mergeCell ref="DP7:DV7"/>
-    <mergeCell ref="DW7:EC7"/>
-    <mergeCell ref="ED7:EJ7"/>
     <mergeCell ref="AX7:BD7"/>
     <mergeCell ref="BL7:BR7"/>
     <mergeCell ref="A1:G2"/>
@@ -5853,44 +7691,56 @@
     <mergeCell ref="AC7:AI7"/>
     <mergeCell ref="AJ7:AP7"/>
     <mergeCell ref="AQ7:AW7"/>
+    <mergeCell ref="EK7:EQ7"/>
+    <mergeCell ref="BE7:BK7"/>
+    <mergeCell ref="BS7:BY7"/>
+    <mergeCell ref="BZ7:CF7"/>
+    <mergeCell ref="CG7:CM7"/>
+    <mergeCell ref="CN7:CT7"/>
+    <mergeCell ref="CU7:DA7"/>
+    <mergeCell ref="DB7:DH7"/>
+    <mergeCell ref="DI7:DO7"/>
+    <mergeCell ref="DP7:DV7"/>
+    <mergeCell ref="DW7:EC7"/>
+    <mergeCell ref="ED7:EJ7"/>
   </mergeCells>
-  <conditionalFormatting sqref="B18:D19 B17 D17 B9:G10 B16:D16 E16:F20 B11:F15 G11:G20">
-    <cfRule type="expression" dxfId="19" priority="20">
+  <conditionalFormatting sqref="B18:D19 B17 D17 B9:G10 B16:D16 E16:F31 B11:F15 B20:C20 G11:G31 B21:D30">
+    <cfRule type="expression" dxfId="0" priority="21">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H9:BD19 BL9:EQ19">
-    <cfRule type="expression" dxfId="18" priority="19">
+  <conditionalFormatting sqref="H9:BD30 BL9:EQ30">
+    <cfRule type="expression" dxfId="25" priority="20">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H9:BD19 BL9:EQ19">
-    <cfRule type="expression" dxfId="17" priority="17">
+  <conditionalFormatting sqref="H9:BD30 BL9:EQ30">
+    <cfRule type="expression" dxfId="24" priority="18">
       <formula>AND(H$8&gt;=$E9,H$8&lt;=$F9)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H9:BD19 BL9:EQ19">
-    <cfRule type="expression" dxfId="16" priority="18">
+  <conditionalFormatting sqref="H9:BD30 BL9:EQ30">
+    <cfRule type="expression" dxfId="23" priority="19">
       <formula>OR(WEEKDAY(H$8,2)=6,WEEKDAY(H$8,2)=7)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BE9:BK19">
-    <cfRule type="expression" dxfId="15" priority="15">
+  <conditionalFormatting sqref="BE9:BK30">
+    <cfRule type="expression" dxfId="22" priority="16">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BE9:BK19">
-    <cfRule type="expression" dxfId="14" priority="13">
+  <conditionalFormatting sqref="BE9:BK30">
+    <cfRule type="expression" dxfId="21" priority="14">
       <formula>AND(BE$8&gt;=$E9,BE$8&lt;=$F9)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BE9:BK19">
-    <cfRule type="expression" dxfId="13" priority="14">
+  <conditionalFormatting sqref="BE9:BK30">
+    <cfRule type="expression" dxfId="20" priority="15">
       <formula>OR(WEEKDAY(BE$8,2)=6,WEEKDAY(BE$8,2)=7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="dataBar" priority="11">
+    <cfRule type="dataBar" priority="12">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5903,43 +7753,48 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B20:D20">
-    <cfRule type="expression" dxfId="12" priority="10">
+  <conditionalFormatting sqref="B31:D31">
+    <cfRule type="expression" dxfId="19" priority="11">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H20:BD20 BL20:EQ20">
-    <cfRule type="expression" dxfId="11" priority="9">
+  <conditionalFormatting sqref="H31:BD31 BL31:EQ31">
+    <cfRule type="expression" dxfId="18" priority="10">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H20:BD20 BL20:EQ20">
-    <cfRule type="expression" dxfId="10" priority="7">
-      <formula>AND(H$8&gt;=$E20,H$8&lt;=$F20)</formula>
+  <conditionalFormatting sqref="H31:BD31 BL31:EQ31">
+    <cfRule type="expression" dxfId="17" priority="8">
+      <formula>AND(H$8&gt;=$E31,H$8&lt;=$F31)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H20:BD20 BL20:EQ20">
-    <cfRule type="expression" dxfId="9" priority="8">
+  <conditionalFormatting sqref="H31:BD31 BL31:EQ31">
+    <cfRule type="expression" dxfId="16" priority="9">
       <formula>OR(WEEKDAY(H$8,2)=6,WEEKDAY(H$8,2)=7)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BE20:BK20">
-    <cfRule type="expression" dxfId="8" priority="5">
+  <conditionalFormatting sqref="BE31:BK31">
+    <cfRule type="expression" dxfId="15" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BE20:BK20">
-    <cfRule type="expression" dxfId="7" priority="3">
-      <formula>AND(BE$8&gt;=$E20,BE$8&lt;=$F20)</formula>
+  <conditionalFormatting sqref="BE31:BK31">
+    <cfRule type="expression" dxfId="14" priority="4">
+      <formula>AND(BE$8&gt;=$E31,BE$8&lt;=$F31)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BE20:BK20">
-    <cfRule type="expression" dxfId="6" priority="4">
+  <conditionalFormatting sqref="BE31:BK31">
+    <cfRule type="expression" dxfId="13" priority="5">
       <formula>OR(WEEKDAY(BE$8,2)=6,WEEKDAY(BE$8,2)=7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="12" priority="2">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D20">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5965,7 +7820,7 @@
           <xm:sqref>C6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="16" id="{A4E1E301-260B-439C-8FA5-07AD136299B7}">
+          <x14:cfRule type="expression" priority="17" id="{A4E1E301-260B-439C-8FA5-07AD136299B7}">
             <xm:f>AND(H$8&lt;=CÁLCULOS!$B3,H$8&gt;=$E9,CÁLCULOS!$A3&gt;=1)</xm:f>
             <x14:dxf>
               <fill>
@@ -5978,8 +7833,8 @@
           <xm:sqref>H9:EQ16</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="6" id="{26BB7447-3313-4134-A3BE-8E2C5A638A34}">
-            <xm:f>AND(H$8&lt;=CÁLCULOS!$B11,H$8&gt;=$E20,CÁLCULOS!$A11&gt;=1)</xm:f>
+          <x14:cfRule type="expression" priority="7" id="{26BB7447-3313-4134-A3BE-8E2C5A638A34}">
+            <xm:f>AND(H$8&lt;=CÁLCULOS!$B11,H$8&gt;=$E31,CÁLCULOS!$A11&gt;=1)</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -5988,11 +7843,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>H20:BD20 BL20:EQ20</xm:sqref>
+          <xm:sqref>H31:BD31 BL31:EQ31</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="2" id="{4896A4C4-8F9E-4217-962B-723F1989E39D}">
-            <xm:f>AND(BE$8&lt;=CÁLCULOS!$B11,BE$8&gt;=$E20,CÁLCULOS!$A11&gt;=1)</xm:f>
+          <x14:cfRule type="expression" priority="3" id="{4896A4C4-8F9E-4217-962B-723F1989E39D}">
+            <xm:f>AND(BE$8&lt;=CÁLCULOS!$B11,BE$8&gt;=$E31,CÁLCULOS!$A11&gt;=1)</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -6001,10 +7856,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>BE20:BK20</xm:sqref>
+          <xm:sqref>BE31:BK31</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="22" id="{A4E1E301-260B-439C-8FA5-07AD136299B7}">
+          <x14:cfRule type="expression" priority="23" id="{A4E1E301-260B-439C-8FA5-07AD136299B7}">
             <xm:f>AND(H$8&lt;=CÁLCULOS!$B10,H$8&gt;=$E17,CÁLCULOS!$A10&gt;=1)</xm:f>
             <x14:dxf>
               <fill>
@@ -6017,7 +7872,7 @@
           <xm:sqref>H17:EQ17</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="24" id="{26BB7447-3313-4134-A3BE-8E2C5A638A34}">
+          <x14:cfRule type="expression" priority="25" id="{26BB7447-3313-4134-A3BE-8E2C5A638A34}">
             <xm:f>AND(H$8&lt;=CÁLCULOS!$B10,H$8&gt;=$E18,CÁLCULOS!$A10&gt;=1)</xm:f>
             <x14:dxf>
               <fill>
@@ -6027,7 +7882,72 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>H18:EQ19</xm:sqref>
+          <xm:sqref>H18:EQ20</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="30" id="{26BB7447-3313-4134-A3BE-8E2C5A638A34}">
+            <xm:f>AND(H$8&lt;=CÁLCULOS!$B12,H$8&gt;=$E26,CÁLCULOS!$A12&gt;=1)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H26:EQ27</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="35" id="{26BB7447-3313-4134-A3BE-8E2C5A638A34}">
+            <xm:f>AND(H$8&lt;=CÁLCULOS!$B12,H$8&gt;=$E21,CÁLCULOS!$A12&gt;=1)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H21:EQ25</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="41" id="{26BB7447-3313-4134-A3BE-8E2C5A638A34}">
+            <xm:f>AND(H$8&lt;=CÁLCULOS!$B13,H$8&gt;=$E30,CÁLCULOS!$A13&gt;=1)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H30:EQ30</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="47" id="{26BB7447-3313-4134-A3BE-8E2C5A638A34}">
+            <xm:f>AND(H$8&lt;=CÁLCULOS!$B13,H$8&gt;=$E29,CÁLCULOS!$A13&gt;=1)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H29:EQ29</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="53" id="{26BB7447-3313-4134-A3BE-8E2C5A638A34}">
+            <xm:f>AND(H$8&lt;=CÁLCULOS!$B13,H$8&gt;=$E28,CÁLCULOS!$A13&gt;=1)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H28:EQ28</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -6071,11 +7991,11 @@
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>'COM FÓRMULAS'!D11*'COM FÓRMULAS'!G11</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" s="23">
         <f>IFERROR(WORKDAY('COM FÓRMULAS'!E11,CÁLCULOS!A5-1),"-")</f>
-        <v>44651</v>
+        <v>44652</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -6101,11 +8021,11 @@
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <f>'COM FÓRMULAS'!D14*'COM FÓRMULAS'!G14</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B8" s="23">
         <f>IFERROR(WORKDAY('COM FÓRMULAS'!E14,CÁLCULOS!A8-1),"-")</f>
-        <v>44662</v>
+        <v>44663</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -6130,121 +8050,121 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
-        <f>'COM FÓRMULAS'!D20*'COM FÓRMULAS'!G20</f>
-        <v>1</v>
+        <f>'COM FÓRMULAS'!D31*'COM FÓRMULAS'!G31</f>
+        <v>0</v>
       </c>
       <c r="B11" s="23">
-        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E20,CÁLCULOS!A11-1),"-")</f>
-        <v>44669</v>
+        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E31,CÁLCULOS!A11-1),"-")</f>
+        <v>44697</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
-        <f>'COM FÓRMULAS'!D21*'COM FÓRMULAS'!G21</f>
+        <f>'COM FÓRMULAS'!D32*'COM FÓRMULAS'!G32</f>
         <v>0</v>
       </c>
       <c r="B12" s="23" t="str">
-        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E21,CÁLCULOS!A12-1),"-")</f>
+        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E32,CÁLCULOS!A12-1),"-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
-        <f>'COM FÓRMULAS'!D22*'COM FÓRMULAS'!G22</f>
+        <f>'COM FÓRMULAS'!D33*'COM FÓRMULAS'!G33</f>
         <v>0</v>
       </c>
       <c r="B13" s="23" t="str">
-        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E22,CÁLCULOS!A13-1),"-")</f>
+        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E33,CÁLCULOS!A13-1),"-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
-        <f>'COM FÓRMULAS'!D23*'COM FÓRMULAS'!G23</f>
+        <f>'COM FÓRMULAS'!D34*'COM FÓRMULAS'!G34</f>
         <v>0</v>
       </c>
       <c r="B14" s="23" t="str">
-        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E23,CÁLCULOS!A14-1),"-")</f>
+        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E34,CÁLCULOS!A14-1),"-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
-        <f>'COM FÓRMULAS'!D24*'COM FÓRMULAS'!G24</f>
+        <f>'COM FÓRMULAS'!D35*'COM FÓRMULAS'!G35</f>
         <v>0</v>
       </c>
       <c r="B15" s="23" t="str">
-        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E24,CÁLCULOS!A15-1),"-")</f>
+        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E35,CÁLCULOS!A15-1),"-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
-        <f>'COM FÓRMULAS'!D25*'COM FÓRMULAS'!G25</f>
+        <f>'COM FÓRMULAS'!D36*'COM FÓRMULAS'!G36</f>
         <v>0</v>
       </c>
       <c r="B16" s="23" t="str">
-        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E25,CÁLCULOS!A16-1),"-")</f>
+        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E36,CÁLCULOS!A16-1),"-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
-        <f>'COM FÓRMULAS'!D26*'COM FÓRMULAS'!G26</f>
+        <f>'COM FÓRMULAS'!D37*'COM FÓRMULAS'!G37</f>
         <v>0</v>
       </c>
       <c r="B17" s="23" t="str">
-        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E26,CÁLCULOS!A17-1),"-")</f>
+        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E37,CÁLCULOS!A17-1),"-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
-        <f>'COM FÓRMULAS'!D27*'COM FÓRMULAS'!G27</f>
+        <f>'COM FÓRMULAS'!D38*'COM FÓRMULAS'!G38</f>
         <v>0</v>
       </c>
       <c r="B18" s="23" t="str">
-        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E27,CÁLCULOS!A18-1),"-")</f>
+        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E38,CÁLCULOS!A18-1),"-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
-        <f>'COM FÓRMULAS'!D28*'COM FÓRMULAS'!G28</f>
+        <f>'COM FÓRMULAS'!D39*'COM FÓRMULAS'!G39</f>
         <v>0</v>
       </c>
       <c r="B19" s="23" t="str">
-        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E28,CÁLCULOS!A19-1),"-")</f>
+        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E39,CÁLCULOS!A19-1),"-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
-        <f>'COM FÓRMULAS'!D29*'COM FÓRMULAS'!G29</f>
+        <f>'COM FÓRMULAS'!D40*'COM FÓRMULAS'!G40</f>
         <v>0</v>
       </c>
       <c r="B20" s="23" t="str">
-        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E29,CÁLCULOS!A20-1),"-")</f>
+        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E40,CÁLCULOS!A20-1),"-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
-        <f>'COM FÓRMULAS'!D30*'COM FÓRMULAS'!G30</f>
+        <f>'COM FÓRMULAS'!D41*'COM FÓRMULAS'!G41</f>
         <v>0</v>
       </c>
       <c r="B21" s="23" t="str">
-        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E30,CÁLCULOS!A21-1),"-")</f>
+        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E41,CÁLCULOS!A21-1),"-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
-        <f>'COM FÓRMULAS'!D31*'COM FÓRMULAS'!G31</f>
+        <f>'COM FÓRMULAS'!D42*'COM FÓRMULAS'!G42</f>
         <v>0</v>
       </c>
       <c r="B22" s="23" t="str">
-        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E31,CÁLCULOS!A22-1),"-")</f>
+        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E42,CÁLCULOS!A22-1),"-")</f>
         <v>-</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Subindo alterações no gráfico de GANTT e atualização do Product Backlog
</commit_message>
<xml_diff>
--- a/Documentação/Gráficos/Gráfico de GANTT.xlsx
+++ b/Documentação/Gráficos/Gráfico de GANTT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITHUB\Documentos\Documentação\Gráficos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367E3731-C23C-4A3B-82AD-E63FF2E267A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D706C741-F2F6-4CF0-ABC9-8BB247A807C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="461" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>#</t>
   </si>
@@ -129,10 +129,13 @@
     <t>Documento de Layout de importação</t>
   </si>
   <si>
-    <t xml:space="preserve">Importação dos dados do arquivo texto </t>
+    <t>Testes unitários (Alinhado com Yoshi</t>
   </si>
   <si>
-    <t>Testes unitários (Alinhado com Yoshi</t>
+    <t xml:space="preserve">Importação de dados do arquivo texto </t>
+  </si>
+  <si>
+    <t>Implementação de fila</t>
   </si>
 </sst>
 </file>
@@ -551,6 +554,9 @@
     <xf numFmtId="9" fontId="12" fillId="5" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="7" fillId="6" borderId="3" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -584,9 +590,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Bom" xfId="2" builtinId="26"/>
@@ -599,39 +602,11 @@
     <cellStyle name="Ruim" xfId="3" builtinId="27"/>
     <cellStyle name="Saída" xfId="5" builtinId="21"/>
   </cellStyles>
-  <dxfs count="31">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="32">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -681,6 +656,34 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -772,6 +775,13 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1027,7 +1037,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.34285714285714286</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2107,86 +2117,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:63" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H1" s="28">
+      <c r="H1" s="29">
         <f>E3</f>
         <v>42492</v>
       </c>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28">
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29">
         <f>H1+7</f>
         <v>42499</v>
       </c>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28">
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29">
         <f>O1+7</f>
         <v>42506</v>
       </c>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="28">
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="29"/>
+      <c r="AC1" s="29">
         <f>V1+7</f>
         <v>42513</v>
       </c>
-      <c r="AD1" s="28"/>
-      <c r="AE1" s="28"/>
-      <c r="AF1" s="28"/>
-      <c r="AG1" s="28"/>
-      <c r="AH1" s="28"/>
-      <c r="AI1" s="28"/>
-      <c r="AJ1" s="28">
+      <c r="AD1" s="29"/>
+      <c r="AE1" s="29"/>
+      <c r="AF1" s="29"/>
+      <c r="AG1" s="29"/>
+      <c r="AH1" s="29"/>
+      <c r="AI1" s="29"/>
+      <c r="AJ1" s="29">
         <f>AC1+7</f>
         <v>42520</v>
       </c>
-      <c r="AK1" s="28"/>
-      <c r="AL1" s="28"/>
-      <c r="AM1" s="28"/>
-      <c r="AN1" s="28"/>
-      <c r="AO1" s="28"/>
-      <c r="AP1" s="28"/>
-      <c r="AQ1" s="28">
+      <c r="AK1" s="29"/>
+      <c r="AL1" s="29"/>
+      <c r="AM1" s="29"/>
+      <c r="AN1" s="29"/>
+      <c r="AO1" s="29"/>
+      <c r="AP1" s="29"/>
+      <c r="AQ1" s="29">
         <f>AJ1+7</f>
         <v>42527</v>
       </c>
-      <c r="AR1" s="28"/>
-      <c r="AS1" s="28"/>
-      <c r="AT1" s="28"/>
-      <c r="AU1" s="28"/>
-      <c r="AV1" s="28"/>
-      <c r="AW1" s="28"/>
-      <c r="AX1" s="28">
+      <c r="AR1" s="29"/>
+      <c r="AS1" s="29"/>
+      <c r="AT1" s="29"/>
+      <c r="AU1" s="29"/>
+      <c r="AV1" s="29"/>
+      <c r="AW1" s="29"/>
+      <c r="AX1" s="29">
         <f>AQ1+7</f>
         <v>42534</v>
       </c>
-      <c r="AY1" s="29"/>
-      <c r="AZ1" s="29"/>
-      <c r="BA1" s="29"/>
-      <c r="BB1" s="29"/>
-      <c r="BC1" s="29"/>
-      <c r="BD1" s="29"/>
-      <c r="BE1" s="28">
+      <c r="AY1" s="30"/>
+      <c r="AZ1" s="30"/>
+      <c r="BA1" s="30"/>
+      <c r="BB1" s="30"/>
+      <c r="BC1" s="30"/>
+      <c r="BD1" s="30"/>
+      <c r="BE1" s="29">
         <f>AX1+7</f>
         <v>42541</v>
       </c>
-      <c r="BF1" s="29"/>
-      <c r="BG1" s="29"/>
-      <c r="BH1" s="29"/>
-      <c r="BI1" s="29"/>
-      <c r="BJ1" s="29"/>
-      <c r="BK1" s="29"/>
+      <c r="BF1" s="30"/>
+      <c r="BG1" s="30"/>
+      <c r="BH1" s="30"/>
+      <c r="BI1" s="30"/>
+      <c r="BJ1" s="30"/>
+      <c r="BK1" s="30"/>
     </row>
     <row r="2" spans="1:63" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
@@ -3070,27 +3080,27 @@
     <mergeCell ref="AJ1:AP1"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:B10 D3:G9 D10 G10">
-    <cfRule type="expression" dxfId="30" priority="5">
+    <cfRule type="expression" dxfId="31" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:BK10">
-    <cfRule type="expression" dxfId="29" priority="4">
+    <cfRule type="expression" dxfId="30" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C9">
-    <cfRule type="expression" dxfId="28" priority="3">
+    <cfRule type="expression" dxfId="29" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="27" priority="2">
+    <cfRule type="expression" dxfId="28" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10:F10">
-    <cfRule type="expression" dxfId="26" priority="1">
+    <cfRule type="expression" dxfId="27" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3101,13 +3111,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:EQ35"/>
+  <dimension ref="A1:EQ36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="8" topLeftCell="AV24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="8" topLeftCell="H27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D31" sqref="D31"/>
+      <selection pane="bottomRight" activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3122,266 +3132,266 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:147" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
     </row>
     <row r="2" spans="1:147" x14ac:dyDescent="0.3">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
     </row>
     <row r="4" spans="1:147" s="2" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="32"/>
-      <c r="F4" s="35">
+      <c r="E4" s="33"/>
+      <c r="F4" s="36">
         <v>44641</v>
       </c>
-      <c r="G4" s="35"/>
+      <c r="G4" s="36"/>
     </row>
     <row r="5" spans="1:147" s="2" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="38"/>
-      <c r="D5" s="33" t="s">
+      <c r="C5" s="39"/>
+      <c r="D5" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="33"/>
-      <c r="F5" s="36">
+      <c r="E5" s="34"/>
+      <c r="F5" s="37">
         <f ca="1">TODAY()</f>
         <v>44689</v>
       </c>
-      <c r="G5" s="36"/>
+      <c r="G5" s="37"/>
     </row>
     <row r="6" spans="1:147" s="2" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="27">
-        <f>(SUM(CÁLCULOS!A3:A22)/SUM('COM FÓRMULAS'!D9:D31))</f>
-        <v>0.34285714285714286</v>
-      </c>
-      <c r="D6" s="34" t="s">
+        <f>(SUM(CÁLCULOS!A3:A22)/SUM('COM FÓRMULAS'!D9:D32))</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D6" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="34"/>
-      <c r="F6" s="37">
-        <f>(F31-E9)+1</f>
+      <c r="E6" s="35"/>
+      <c r="F6" s="38">
+        <f>(F32-E9)+1</f>
         <v>54</v>
       </c>
-      <c r="G6" s="37"/>
+      <c r="G6" s="38"/>
     </row>
     <row r="7" spans="1:147" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H7" s="28">
+      <c r="H7" s="29">
         <f>E9</f>
         <v>44645</v>
       </c>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="28"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="28">
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="29">
         <f>H7+7</f>
         <v>44652</v>
       </c>
-      <c r="P7" s="28"/>
-      <c r="Q7" s="28"/>
-      <c r="R7" s="28"/>
-      <c r="S7" s="28"/>
-      <c r="T7" s="28"/>
-      <c r="U7" s="28"/>
-      <c r="V7" s="28">
+      <c r="P7" s="29"/>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="29"/>
+      <c r="S7" s="29"/>
+      <c r="T7" s="29"/>
+      <c r="U7" s="29"/>
+      <c r="V7" s="29">
         <f>O7+7</f>
         <v>44659</v>
       </c>
-      <c r="W7" s="28"/>
-      <c r="X7" s="28"/>
-      <c r="Y7" s="28"/>
-      <c r="Z7" s="28"/>
-      <c r="AA7" s="28"/>
-      <c r="AB7" s="28"/>
-      <c r="AC7" s="28">
+      <c r="W7" s="29"/>
+      <c r="X7" s="29"/>
+      <c r="Y7" s="29"/>
+      <c r="Z7" s="29"/>
+      <c r="AA7" s="29"/>
+      <c r="AB7" s="29"/>
+      <c r="AC7" s="29">
         <f>V7+7</f>
         <v>44666</v>
       </c>
-      <c r="AD7" s="28"/>
-      <c r="AE7" s="28"/>
-      <c r="AF7" s="28"/>
-      <c r="AG7" s="28"/>
-      <c r="AH7" s="28"/>
-      <c r="AI7" s="28"/>
-      <c r="AJ7" s="28">
+      <c r="AD7" s="29"/>
+      <c r="AE7" s="29"/>
+      <c r="AF7" s="29"/>
+      <c r="AG7" s="29"/>
+      <c r="AH7" s="29"/>
+      <c r="AI7" s="29"/>
+      <c r="AJ7" s="29">
         <f>AC7+7</f>
         <v>44673</v>
       </c>
-      <c r="AK7" s="28"/>
-      <c r="AL7" s="28"/>
-      <c r="AM7" s="28"/>
-      <c r="AN7" s="28"/>
-      <c r="AO7" s="28"/>
-      <c r="AP7" s="28"/>
-      <c r="AQ7" s="28">
+      <c r="AK7" s="29"/>
+      <c r="AL7" s="29"/>
+      <c r="AM7" s="29"/>
+      <c r="AN7" s="29"/>
+      <c r="AO7" s="29"/>
+      <c r="AP7" s="29"/>
+      <c r="AQ7" s="29">
         <f>AJ7+7</f>
         <v>44680</v>
       </c>
-      <c r="AR7" s="28"/>
-      <c r="AS7" s="28"/>
-      <c r="AT7" s="28"/>
-      <c r="AU7" s="28"/>
-      <c r="AV7" s="28"/>
-      <c r="AW7" s="28"/>
-      <c r="AX7" s="28">
+      <c r="AR7" s="29"/>
+      <c r="AS7" s="29"/>
+      <c r="AT7" s="29"/>
+      <c r="AU7" s="29"/>
+      <c r="AV7" s="29"/>
+      <c r="AW7" s="29"/>
+      <c r="AX7" s="29">
         <f>AQ7+7</f>
         <v>44687</v>
       </c>
-      <c r="AY7" s="29"/>
-      <c r="AZ7" s="29"/>
-      <c r="BA7" s="29"/>
-      <c r="BB7" s="29"/>
-      <c r="BC7" s="29"/>
-      <c r="BD7" s="29"/>
-      <c r="BE7" s="28">
+      <c r="AY7" s="30"/>
+      <c r="AZ7" s="30"/>
+      <c r="BA7" s="30"/>
+      <c r="BB7" s="30"/>
+      <c r="BC7" s="30"/>
+      <c r="BD7" s="30"/>
+      <c r="BE7" s="29">
         <f>AX7+7</f>
         <v>44694</v>
       </c>
-      <c r="BF7" s="29"/>
-      <c r="BG7" s="29"/>
-      <c r="BH7" s="29"/>
-      <c r="BI7" s="29"/>
-      <c r="BJ7" s="29"/>
-      <c r="BK7" s="29"/>
-      <c r="BL7" s="28">
+      <c r="BF7" s="30"/>
+      <c r="BG7" s="30"/>
+      <c r="BH7" s="30"/>
+      <c r="BI7" s="30"/>
+      <c r="BJ7" s="30"/>
+      <c r="BK7" s="30"/>
+      <c r="BL7" s="29">
         <f>BE7+7</f>
         <v>44701</v>
       </c>
-      <c r="BM7" s="29"/>
-      <c r="BN7" s="29"/>
-      <c r="BO7" s="29"/>
-      <c r="BP7" s="29"/>
-      <c r="BQ7" s="29"/>
-      <c r="BR7" s="29"/>
-      <c r="BS7" s="28">
+      <c r="BM7" s="30"/>
+      <c r="BN7" s="30"/>
+      <c r="BO7" s="30"/>
+      <c r="BP7" s="30"/>
+      <c r="BQ7" s="30"/>
+      <c r="BR7" s="30"/>
+      <c r="BS7" s="29">
         <f>BL7+7</f>
         <v>44708</v>
       </c>
-      <c r="BT7" s="29"/>
-      <c r="BU7" s="29"/>
-      <c r="BV7" s="29"/>
-      <c r="BW7" s="29"/>
-      <c r="BX7" s="29"/>
-      <c r="BY7" s="29"/>
-      <c r="BZ7" s="28">
+      <c r="BT7" s="30"/>
+      <c r="BU7" s="30"/>
+      <c r="BV7" s="30"/>
+      <c r="BW7" s="30"/>
+      <c r="BX7" s="30"/>
+      <c r="BY7" s="30"/>
+      <c r="BZ7" s="29">
         <f t="shared" ref="BZ7" si="0">BS7+7</f>
         <v>44715</v>
       </c>
-      <c r="CA7" s="29"/>
-      <c r="CB7" s="29"/>
-      <c r="CC7" s="29"/>
-      <c r="CD7" s="29"/>
-      <c r="CE7" s="29"/>
-      <c r="CF7" s="29"/>
-      <c r="CG7" s="28">
+      <c r="CA7" s="30"/>
+      <c r="CB7" s="30"/>
+      <c r="CC7" s="30"/>
+      <c r="CD7" s="30"/>
+      <c r="CE7" s="30"/>
+      <c r="CF7" s="30"/>
+      <c r="CG7" s="29">
         <f t="shared" ref="CG7" si="1">BZ7+7</f>
         <v>44722</v>
       </c>
-      <c r="CH7" s="29"/>
-      <c r="CI7" s="29"/>
-      <c r="CJ7" s="29"/>
-      <c r="CK7" s="29"/>
-      <c r="CL7" s="29"/>
-      <c r="CM7" s="29"/>
-      <c r="CN7" s="28">
+      <c r="CH7" s="30"/>
+      <c r="CI7" s="30"/>
+      <c r="CJ7" s="30"/>
+      <c r="CK7" s="30"/>
+      <c r="CL7" s="30"/>
+      <c r="CM7" s="30"/>
+      <c r="CN7" s="29">
         <f t="shared" ref="CN7" si="2">CG7+7</f>
         <v>44729</v>
       </c>
-      <c r="CO7" s="29"/>
-      <c r="CP7" s="29"/>
-      <c r="CQ7" s="29"/>
-      <c r="CR7" s="29"/>
-      <c r="CS7" s="29"/>
-      <c r="CT7" s="29"/>
-      <c r="CU7" s="28">
+      <c r="CO7" s="30"/>
+      <c r="CP7" s="30"/>
+      <c r="CQ7" s="30"/>
+      <c r="CR7" s="30"/>
+      <c r="CS7" s="30"/>
+      <c r="CT7" s="30"/>
+      <c r="CU7" s="29">
         <f t="shared" ref="CU7" si="3">CN7+7</f>
         <v>44736</v>
       </c>
-      <c r="CV7" s="29"/>
-      <c r="CW7" s="29"/>
-      <c r="CX7" s="29"/>
-      <c r="CY7" s="29"/>
-      <c r="CZ7" s="29"/>
-      <c r="DA7" s="29"/>
-      <c r="DB7" s="28">
+      <c r="CV7" s="30"/>
+      <c r="CW7" s="30"/>
+      <c r="CX7" s="30"/>
+      <c r="CY7" s="30"/>
+      <c r="CZ7" s="30"/>
+      <c r="DA7" s="30"/>
+      <c r="DB7" s="29">
         <f t="shared" ref="DB7" si="4">CU7+7</f>
         <v>44743</v>
       </c>
-      <c r="DC7" s="29"/>
-      <c r="DD7" s="29"/>
-      <c r="DE7" s="29"/>
-      <c r="DF7" s="29"/>
-      <c r="DG7" s="29"/>
-      <c r="DH7" s="29"/>
-      <c r="DI7" s="28">
+      <c r="DC7" s="30"/>
+      <c r="DD7" s="30"/>
+      <c r="DE7" s="30"/>
+      <c r="DF7" s="30"/>
+      <c r="DG7" s="30"/>
+      <c r="DH7" s="30"/>
+      <c r="DI7" s="29">
         <f t="shared" ref="DI7" si="5">DB7+7</f>
         <v>44750</v>
       </c>
-      <c r="DJ7" s="29"/>
-      <c r="DK7" s="29"/>
-      <c r="DL7" s="29"/>
-      <c r="DM7" s="29"/>
-      <c r="DN7" s="29"/>
-      <c r="DO7" s="29"/>
-      <c r="DP7" s="28">
+      <c r="DJ7" s="30"/>
+      <c r="DK7" s="30"/>
+      <c r="DL7" s="30"/>
+      <c r="DM7" s="30"/>
+      <c r="DN7" s="30"/>
+      <c r="DO7" s="30"/>
+      <c r="DP7" s="29">
         <f t="shared" ref="DP7" si="6">DI7+7</f>
         <v>44757</v>
       </c>
-      <c r="DQ7" s="29"/>
-      <c r="DR7" s="29"/>
-      <c r="DS7" s="29"/>
-      <c r="DT7" s="29"/>
-      <c r="DU7" s="29"/>
-      <c r="DV7" s="29"/>
-      <c r="DW7" s="28">
+      <c r="DQ7" s="30"/>
+      <c r="DR7" s="30"/>
+      <c r="DS7" s="30"/>
+      <c r="DT7" s="30"/>
+      <c r="DU7" s="30"/>
+      <c r="DV7" s="30"/>
+      <c r="DW7" s="29">
         <f t="shared" ref="DW7" si="7">DP7+7</f>
         <v>44764</v>
       </c>
-      <c r="DX7" s="29"/>
-      <c r="DY7" s="29"/>
-      <c r="DZ7" s="29"/>
-      <c r="EA7" s="29"/>
-      <c r="EB7" s="29"/>
-      <c r="EC7" s="29"/>
-      <c r="ED7" s="28">
+      <c r="DX7" s="30"/>
+      <c r="DY7" s="30"/>
+      <c r="DZ7" s="30"/>
+      <c r="EA7" s="30"/>
+      <c r="EB7" s="30"/>
+      <c r="EC7" s="30"/>
+      <c r="ED7" s="29">
         <f t="shared" ref="ED7" si="8">DW7+7</f>
         <v>44771</v>
       </c>
-      <c r="EE7" s="29"/>
-      <c r="EF7" s="29"/>
-      <c r="EG7" s="29"/>
-      <c r="EH7" s="29"/>
-      <c r="EI7" s="29"/>
-      <c r="EJ7" s="29"/>
-      <c r="EK7" s="28">
+      <c r="EE7" s="30"/>
+      <c r="EF7" s="30"/>
+      <c r="EG7" s="30"/>
+      <c r="EH7" s="30"/>
+      <c r="EI7" s="30"/>
+      <c r="EJ7" s="30"/>
+      <c r="EK7" s="29">
         <f t="shared" ref="EK7" si="9">ED7+7</f>
         <v>44778</v>
       </c>
-      <c r="EL7" s="29"/>
-      <c r="EM7" s="29"/>
-      <c r="EN7" s="29"/>
-      <c r="EO7" s="29"/>
-      <c r="EP7" s="29"/>
-      <c r="EQ7" s="29"/>
+      <c r="EL7" s="30"/>
+      <c r="EM7" s="30"/>
+      <c r="EN7" s="30"/>
+      <c r="EO7" s="30"/>
+      <c r="EP7" s="30"/>
+      <c r="EQ7" s="30"/>
     </row>
     <row r="8" spans="1:147" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
@@ -5749,7 +5759,7 @@
         <v>44669</v>
       </c>
       <c r="F20" s="13">
-        <f>WORKDAY(E20,(D20-1))</f>
+        <f t="shared" ref="F20:F32" si="103">WORKDAY(E20,(D20-1))</f>
         <v>44670</v>
       </c>
       <c r="G20" s="10">
@@ -5900,7 +5910,7 @@
       <c r="B21" s="7">
         <v>13</v>
       </c>
-      <c r="C21" s="39" t="s">
+      <c r="C21" s="28" t="s">
         <v>26</v>
       </c>
       <c r="D21" s="26">
@@ -5910,7 +5920,7 @@
         <v>44687</v>
       </c>
       <c r="F21" s="13">
-        <f>WORKDAY(E21,(D21-1))</f>
+        <f t="shared" si="103"/>
         <v>44687</v>
       </c>
       <c r="G21" s="10">
@@ -6071,7 +6081,7 @@
         <v>44688</v>
       </c>
       <c r="F22" s="13">
-        <f>WORKDAY(E22,(D22-1))</f>
+        <f t="shared" si="103"/>
         <v>44688</v>
       </c>
       <c r="G22" s="10">
@@ -6218,12 +6228,12 @@
       <c r="EP22" s="19"/>
       <c r="EQ22" s="19"/>
     </row>
-    <row r="23" spans="2:147" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:147" s="2" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="7">
         <v>15</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D23" s="26">
         <v>1</v>
@@ -6232,11 +6242,11 @@
         <v>44688</v>
       </c>
       <c r="F23" s="13">
-        <f>WORKDAY(E23,(D23-1))</f>
+        <f t="shared" si="103"/>
         <v>44688</v>
       </c>
       <c r="G23" s="10">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H23" s="19"/>
       <c r="I23" s="19"/>
@@ -6384,17 +6394,17 @@
         <v>16</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D24" s="26">
         <v>1</v>
       </c>
       <c r="E24" s="9">
-        <v>44689</v>
+        <v>44688</v>
       </c>
       <c r="F24" s="13">
-        <f>WORKDAY(E24,(D24-1))</f>
-        <v>44689</v>
+        <f t="shared" si="103"/>
+        <v>44688</v>
       </c>
       <c r="G24" s="10">
         <v>0</v>
@@ -6545,20 +6555,20 @@
         <v>17</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D25" s="26">
         <v>1</v>
       </c>
       <c r="E25" s="9">
-        <v>44690</v>
+        <v>44689</v>
       </c>
       <c r="F25" s="13">
-        <f>WORKDAY(E25,(D25-1))</f>
-        <v>44690</v>
+        <f t="shared" si="103"/>
+        <v>44689</v>
       </c>
       <c r="G25" s="10">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H25" s="19"/>
       <c r="I25" s="19"/>
@@ -6706,20 +6716,20 @@
         <v>18</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D26" s="26">
         <v>1</v>
       </c>
       <c r="E26" s="9">
-        <v>44692</v>
+        <v>44690</v>
       </c>
       <c r="F26" s="13">
-        <f>WORKDAY(E26,(D26-1))</f>
-        <v>44692</v>
+        <f t="shared" si="103"/>
+        <v>44690</v>
       </c>
       <c r="G26" s="10">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H26" s="19"/>
       <c r="I26" s="19"/>
@@ -6867,17 +6877,17 @@
         <v>19</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D27" s="26">
         <v>1</v>
       </c>
       <c r="E27" s="9">
-        <v>44693</v>
+        <v>44692</v>
       </c>
       <c r="F27" s="13">
-        <f>WORKDAY(E27,(D27-1))</f>
-        <v>44693</v>
+        <f t="shared" si="103"/>
+        <v>44692</v>
       </c>
       <c r="G27" s="10">
         <v>0</v>
@@ -7028,17 +7038,17 @@
         <v>20</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D28" s="26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E28" s="9">
-        <v>44694</v>
+        <v>44693</v>
       </c>
       <c r="F28" s="13">
-        <f>WORKDAY(E28,(D28-1))</f>
-        <v>44697</v>
+        <f t="shared" si="103"/>
+        <v>44693</v>
       </c>
       <c r="G28" s="10">
         <v>0</v>
@@ -7189,17 +7199,17 @@
         <v>21</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="D29" s="26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E29" s="9">
-        <v>44695</v>
+        <v>44694</v>
       </c>
       <c r="F29" s="13">
-        <f>WORKDAY(E29,(D29-1))</f>
-        <v>44698</v>
+        <f t="shared" si="103"/>
+        <v>44697</v>
       </c>
       <c r="G29" s="10">
         <v>0</v>
@@ -7350,16 +7360,16 @@
         <v>22</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D30" s="26">
         <v>3</v>
       </c>
       <c r="E30" s="9">
-        <v>44696</v>
+        <v>44695</v>
       </c>
       <c r="F30" s="13">
-        <f>WORKDAY(E30,(D30-1))</f>
+        <f t="shared" si="103"/>
         <v>44698</v>
       </c>
       <c r="G30" s="10">
@@ -7511,16 +7521,16 @@
         <v>23</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D31" s="26">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E31" s="9">
-        <v>44698</v>
+        <v>44696</v>
       </c>
       <c r="F31" s="13">
-        <f>WORKDAY(E31,(D31-1))</f>
+        <f t="shared" si="103"/>
         <v>44698</v>
       </c>
       <c r="G31" s="10">
@@ -7667,14 +7677,187 @@
       <c r="EP31" s="19"/>
       <c r="EQ31" s="19"/>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C34" s="1"/>
+    <row r="32" spans="2:147" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="7">
+        <v>24</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="26">
+        <v>1</v>
+      </c>
+      <c r="E32" s="9">
+        <v>44698</v>
+      </c>
+      <c r="F32" s="13">
+        <f t="shared" si="103"/>
+        <v>44698</v>
+      </c>
+      <c r="G32" s="10">
+        <v>0</v>
+      </c>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
+      <c r="O32" s="19"/>
+      <c r="P32" s="19"/>
+      <c r="Q32" s="19"/>
+      <c r="R32" s="19"/>
+      <c r="S32" s="19"/>
+      <c r="T32" s="19"/>
+      <c r="U32" s="19"/>
+      <c r="V32" s="19"/>
+      <c r="W32" s="19"/>
+      <c r="X32" s="19"/>
+      <c r="Y32" s="19"/>
+      <c r="Z32" s="19"/>
+      <c r="AA32" s="19"/>
+      <c r="AB32" s="19"/>
+      <c r="AC32" s="19"/>
+      <c r="AD32" s="19"/>
+      <c r="AE32" s="19"/>
+      <c r="AF32" s="19"/>
+      <c r="AG32" s="19"/>
+      <c r="AH32" s="19"/>
+      <c r="AI32" s="19"/>
+      <c r="AJ32" s="19"/>
+      <c r="AK32" s="19"/>
+      <c r="AL32" s="19"/>
+      <c r="AM32" s="19"/>
+      <c r="AN32" s="19"/>
+      <c r="AO32" s="19"/>
+      <c r="AP32" s="19"/>
+      <c r="AQ32" s="19"/>
+      <c r="AR32" s="19"/>
+      <c r="AS32" s="19"/>
+      <c r="AT32" s="19"/>
+      <c r="AU32" s="19"/>
+      <c r="AV32" s="19"/>
+      <c r="AW32" s="19"/>
+      <c r="AX32" s="19"/>
+      <c r="AY32" s="19"/>
+      <c r="AZ32" s="19"/>
+      <c r="BA32" s="19"/>
+      <c r="BB32" s="19"/>
+      <c r="BC32" s="19"/>
+      <c r="BD32" s="19"/>
+      <c r="BE32" s="19"/>
+      <c r="BF32" s="19"/>
+      <c r="BG32" s="19"/>
+      <c r="BH32" s="19"/>
+      <c r="BI32" s="19"/>
+      <c r="BJ32" s="19"/>
+      <c r="BK32" s="19"/>
+      <c r="BL32" s="19"/>
+      <c r="BM32" s="19"/>
+      <c r="BN32" s="19"/>
+      <c r="BO32" s="19"/>
+      <c r="BP32" s="19"/>
+      <c r="BQ32" s="19"/>
+      <c r="BR32" s="19"/>
+      <c r="BS32" s="19"/>
+      <c r="BT32" s="19"/>
+      <c r="BU32" s="19"/>
+      <c r="BV32" s="19"/>
+      <c r="BW32" s="19"/>
+      <c r="BX32" s="19"/>
+      <c r="BY32" s="19"/>
+      <c r="BZ32" s="19"/>
+      <c r="CA32" s="19"/>
+      <c r="CB32" s="19"/>
+      <c r="CC32" s="19"/>
+      <c r="CD32" s="19"/>
+      <c r="CE32" s="19"/>
+      <c r="CF32" s="19"/>
+      <c r="CG32" s="19"/>
+      <c r="CH32" s="19"/>
+      <c r="CI32" s="19"/>
+      <c r="CJ32" s="19"/>
+      <c r="CK32" s="19"/>
+      <c r="CL32" s="19"/>
+      <c r="CM32" s="19"/>
+      <c r="CN32" s="19"/>
+      <c r="CO32" s="19"/>
+      <c r="CP32" s="19"/>
+      <c r="CQ32" s="19"/>
+      <c r="CR32" s="19"/>
+      <c r="CS32" s="19"/>
+      <c r="CT32" s="19"/>
+      <c r="CU32" s="19"/>
+      <c r="CV32" s="19"/>
+      <c r="CW32" s="19"/>
+      <c r="CX32" s="19"/>
+      <c r="CY32" s="19"/>
+      <c r="CZ32" s="19"/>
+      <c r="DA32" s="19"/>
+      <c r="DB32" s="19"/>
+      <c r="DC32" s="19"/>
+      <c r="DD32" s="19"/>
+      <c r="DE32" s="19"/>
+      <c r="DF32" s="19"/>
+      <c r="DG32" s="19"/>
+      <c r="DH32" s="19"/>
+      <c r="DI32" s="19"/>
+      <c r="DJ32" s="19"/>
+      <c r="DK32" s="19"/>
+      <c r="DL32" s="19"/>
+      <c r="DM32" s="19"/>
+      <c r="DN32" s="19"/>
+      <c r="DO32" s="19"/>
+      <c r="DP32" s="19"/>
+      <c r="DQ32" s="19"/>
+      <c r="DR32" s="19"/>
+      <c r="DS32" s="19"/>
+      <c r="DT32" s="19"/>
+      <c r="DU32" s="19"/>
+      <c r="DV32" s="19"/>
+      <c r="DW32" s="19"/>
+      <c r="DX32" s="19"/>
+      <c r="DY32" s="19"/>
+      <c r="DZ32" s="19"/>
+      <c r="EA32" s="19"/>
+      <c r="EB32" s="19"/>
+      <c r="EC32" s="19"/>
+      <c r="ED32" s="19"/>
+      <c r="EE32" s="19"/>
+      <c r="EF32" s="19"/>
+      <c r="EG32" s="19"/>
+      <c r="EH32" s="19"/>
+      <c r="EI32" s="19"/>
+      <c r="EJ32" s="19"/>
+      <c r="EK32" s="19"/>
+      <c r="EL32" s="19"/>
+      <c r="EM32" s="19"/>
+      <c r="EN32" s="19"/>
+      <c r="EO32" s="19"/>
+      <c r="EP32" s="19"/>
+      <c r="EQ32" s="19"/>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C35" s="1"/>
     </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C36" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="EK7:EQ7"/>
+    <mergeCell ref="BE7:BK7"/>
+    <mergeCell ref="BS7:BY7"/>
+    <mergeCell ref="BZ7:CF7"/>
+    <mergeCell ref="CG7:CM7"/>
+    <mergeCell ref="CN7:CT7"/>
+    <mergeCell ref="CU7:DA7"/>
+    <mergeCell ref="DB7:DH7"/>
+    <mergeCell ref="DI7:DO7"/>
+    <mergeCell ref="DP7:DV7"/>
+    <mergeCell ref="DW7:EC7"/>
+    <mergeCell ref="ED7:EJ7"/>
     <mergeCell ref="AX7:BD7"/>
     <mergeCell ref="BL7:BR7"/>
     <mergeCell ref="A1:G2"/>
@@ -7691,50 +7874,38 @@
     <mergeCell ref="AC7:AI7"/>
     <mergeCell ref="AJ7:AP7"/>
     <mergeCell ref="AQ7:AW7"/>
-    <mergeCell ref="EK7:EQ7"/>
-    <mergeCell ref="BE7:BK7"/>
-    <mergeCell ref="BS7:BY7"/>
-    <mergeCell ref="BZ7:CF7"/>
-    <mergeCell ref="CG7:CM7"/>
-    <mergeCell ref="CN7:CT7"/>
-    <mergeCell ref="CU7:DA7"/>
-    <mergeCell ref="DB7:DH7"/>
-    <mergeCell ref="DI7:DO7"/>
-    <mergeCell ref="DP7:DV7"/>
-    <mergeCell ref="DW7:EC7"/>
-    <mergeCell ref="ED7:EJ7"/>
   </mergeCells>
-  <conditionalFormatting sqref="B18:D19 B17 D17 B9:G10 B16:D16 E16:F31 B11:F15 B20:C20 G11:G31 B21:D30">
-    <cfRule type="expression" dxfId="0" priority="21">
+  <conditionalFormatting sqref="B18:D19 B17 D17 B9:G10 B16:D16 E16:F32 B11:F15 B20:C20 G11:G32 B21:D31">
+    <cfRule type="expression" dxfId="26" priority="21">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H9:BD30 BL9:EQ30">
+  <conditionalFormatting sqref="H9:BD31 BL9:EQ31">
     <cfRule type="expression" dxfId="25" priority="20">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H9:BD30 BL9:EQ30">
+  <conditionalFormatting sqref="H9:BD31 BL9:EQ31">
     <cfRule type="expression" dxfId="24" priority="18">
       <formula>AND(H$8&gt;=$E9,H$8&lt;=$F9)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H9:BD30 BL9:EQ30">
+  <conditionalFormatting sqref="H9:BD31 BL9:EQ31">
     <cfRule type="expression" dxfId="23" priority="19">
       <formula>OR(WEEKDAY(H$8,2)=6,WEEKDAY(H$8,2)=7)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BE9:BK30">
+  <conditionalFormatting sqref="BE9:BK31">
     <cfRule type="expression" dxfId="22" priority="16">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BE9:BK30">
+  <conditionalFormatting sqref="BE9:BK31">
     <cfRule type="expression" dxfId="21" priority="14">
       <formula>AND(BE$8&gt;=$E9,BE$8&lt;=$F9)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BE9:BK30">
+  <conditionalFormatting sqref="BE9:BK31">
     <cfRule type="expression" dxfId="20" priority="15">
       <formula>OR(WEEKDAY(BE$8,2)=6,WEEKDAY(BE$8,2)=7)</formula>
     </cfRule>
@@ -7753,37 +7924,37 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B31:D31">
+  <conditionalFormatting sqref="B32:D32">
     <cfRule type="expression" dxfId="19" priority="11">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H31:BD31 BL31:EQ31">
+  <conditionalFormatting sqref="H32:BD32 BL32:EQ32">
     <cfRule type="expression" dxfId="18" priority="10">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H31:BD31 BL31:EQ31">
+  <conditionalFormatting sqref="H32:BD32 BL32:EQ32">
     <cfRule type="expression" dxfId="17" priority="8">
-      <formula>AND(H$8&gt;=$E31,H$8&lt;=$F31)</formula>
+      <formula>AND(H$8&gt;=$E32,H$8&lt;=$F32)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H31:BD31 BL31:EQ31">
+  <conditionalFormatting sqref="H32:BD32 BL32:EQ32">
     <cfRule type="expression" dxfId="16" priority="9">
       <formula>OR(WEEKDAY(H$8,2)=6,WEEKDAY(H$8,2)=7)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BE31:BK31">
+  <conditionalFormatting sqref="BE32:BK32">
     <cfRule type="expression" dxfId="15" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BE31:BK31">
+  <conditionalFormatting sqref="BE32:BK32">
     <cfRule type="expression" dxfId="14" priority="4">
-      <formula>AND(BE$8&gt;=$E31,BE$8&lt;=$F31)</formula>
+      <formula>AND(BE$8&gt;=$E32,BE$8&lt;=$F32)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BE31:BK31">
+  <conditionalFormatting sqref="BE32:BK32">
     <cfRule type="expression" dxfId="13" priority="5">
       <formula>OR(WEEKDAY(BE$8,2)=6,WEEKDAY(BE$8,2)=7)</formula>
     </cfRule>
@@ -7794,7 +7965,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="11" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7834,7 +8005,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="7" id="{26BB7447-3313-4134-A3BE-8E2C5A638A34}">
-            <xm:f>AND(H$8&lt;=CÁLCULOS!$B11,H$8&gt;=$E31,CÁLCULOS!$A11&gt;=1)</xm:f>
+            <xm:f>AND(H$8&lt;=CÁLCULOS!$B11,H$8&gt;=$E32,CÁLCULOS!$A11&gt;=1)</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -7843,11 +8014,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>H31:BD31 BL31:EQ31</xm:sqref>
+          <xm:sqref>H32:BD32 BL32:EQ32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="3" id="{4896A4C4-8F9E-4217-962B-723F1989E39D}">
-            <xm:f>AND(BE$8&lt;=CÁLCULOS!$B11,BE$8&gt;=$E31,CÁLCULOS!$A11&gt;=1)</xm:f>
+            <xm:f>AND(BE$8&lt;=CÁLCULOS!$B11,BE$8&gt;=$E32,CÁLCULOS!$A11&gt;=1)</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -7856,7 +8027,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>BE31:BK31</xm:sqref>
+          <xm:sqref>BE32:BK32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="23" id="{A4E1E301-260B-439C-8FA5-07AD136299B7}">
@@ -7885,19 +8056,6 @@
           <xm:sqref>H18:EQ20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="30" id="{26BB7447-3313-4134-A3BE-8E2C5A638A34}">
-            <xm:f>AND(H$8&lt;=CÁLCULOS!$B12,H$8&gt;=$E26,CÁLCULOS!$A12&gt;=1)</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>H26:EQ27</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="35" id="{26BB7447-3313-4134-A3BE-8E2C5A638A34}">
             <xm:f>AND(H$8&lt;=CÁLCULOS!$B12,H$8&gt;=$E21,CÁLCULOS!$A12&gt;=1)</xm:f>
             <x14:dxf>
@@ -7908,10 +8066,23 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>H21:EQ25</xm:sqref>
+          <xm:sqref>H21:EQ23</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="41" id="{26BB7447-3313-4134-A3BE-8E2C5A638A34}">
+            <xm:f>AND(H$8&lt;=CÁLCULOS!$B13,H$8&gt;=$E31,CÁLCULOS!$A13&gt;=1)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H31:EQ31</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="47" id="{26BB7447-3313-4134-A3BE-8E2C5A638A34}">
             <xm:f>AND(H$8&lt;=CÁLCULOS!$B13,H$8&gt;=$E30,CÁLCULOS!$A13&gt;=1)</xm:f>
             <x14:dxf>
               <fill>
@@ -7924,7 +8095,7 @@
           <xm:sqref>H30:EQ30</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="47" id="{26BB7447-3313-4134-A3BE-8E2C5A638A34}">
+          <x14:cfRule type="expression" priority="53" id="{26BB7447-3313-4134-A3BE-8E2C5A638A34}">
             <xm:f>AND(H$8&lt;=CÁLCULOS!$B13,H$8&gt;=$E29,CÁLCULOS!$A13&gt;=1)</xm:f>
             <x14:dxf>
               <fill>
@@ -7937,8 +8108,8 @@
           <xm:sqref>H29:EQ29</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="53" id="{26BB7447-3313-4134-A3BE-8E2C5A638A34}">
-            <xm:f>AND(H$8&lt;=CÁLCULOS!$B13,H$8&gt;=$E28,CÁLCULOS!$A13&gt;=1)</xm:f>
+          <x14:cfRule type="expression" priority="58" id="{26BB7447-3313-4134-A3BE-8E2C5A638A34}">
+            <xm:f>AND(H$8&lt;=CÁLCULOS!$B12,H$8&gt;=$E27,CÁLCULOS!$A12&gt;=1)</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -7947,7 +8118,20 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>H28:EQ28</xm:sqref>
+          <xm:sqref>H27:EQ28</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="60" id="{26BB7447-3313-4134-A3BE-8E2C5A638A34}">
+            <xm:f>AND(H$8&lt;=CÁLCULOS!$B14,H$8&gt;=$E24,CÁLCULOS!$A14&gt;=1)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H24:EQ26</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -8050,121 +8234,121 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
-        <f>'COM FÓRMULAS'!D31*'COM FÓRMULAS'!G31</f>
+        <f>'COM FÓRMULAS'!D32*'COM FÓRMULAS'!G32</f>
         <v>0</v>
       </c>
       <c r="B11" s="23">
-        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E31,CÁLCULOS!A11-1),"-")</f>
+        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E32,CÁLCULOS!A11-1),"-")</f>
         <v>44697</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
-        <f>'COM FÓRMULAS'!D32*'COM FÓRMULAS'!G32</f>
+        <f>'COM FÓRMULAS'!D33*'COM FÓRMULAS'!G33</f>
         <v>0</v>
       </c>
       <c r="B12" s="23" t="str">
-        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E32,CÁLCULOS!A12-1),"-")</f>
+        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E33,CÁLCULOS!A12-1),"-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
-        <f>'COM FÓRMULAS'!D33*'COM FÓRMULAS'!G33</f>
+        <f>'COM FÓRMULAS'!D34*'COM FÓRMULAS'!G34</f>
         <v>0</v>
       </c>
       <c r="B13" s="23" t="str">
-        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E33,CÁLCULOS!A13-1),"-")</f>
+        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E34,CÁLCULOS!A13-1),"-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
-        <f>'COM FÓRMULAS'!D34*'COM FÓRMULAS'!G34</f>
+        <f>'COM FÓRMULAS'!D35*'COM FÓRMULAS'!G35</f>
         <v>0</v>
       </c>
       <c r="B14" s="23" t="str">
-        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E34,CÁLCULOS!A14-1),"-")</f>
+        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E35,CÁLCULOS!A14-1),"-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
-        <f>'COM FÓRMULAS'!D35*'COM FÓRMULAS'!G35</f>
+        <f>'COM FÓRMULAS'!D36*'COM FÓRMULAS'!G36</f>
         <v>0</v>
       </c>
       <c r="B15" s="23" t="str">
-        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E35,CÁLCULOS!A15-1),"-")</f>
+        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E36,CÁLCULOS!A15-1),"-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
-        <f>'COM FÓRMULAS'!D36*'COM FÓRMULAS'!G36</f>
+        <f>'COM FÓRMULAS'!D37*'COM FÓRMULAS'!G37</f>
         <v>0</v>
       </c>
       <c r="B16" s="23" t="str">
-        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E36,CÁLCULOS!A16-1),"-")</f>
+        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E37,CÁLCULOS!A16-1),"-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
-        <f>'COM FÓRMULAS'!D37*'COM FÓRMULAS'!G37</f>
+        <f>'COM FÓRMULAS'!D38*'COM FÓRMULAS'!G38</f>
         <v>0</v>
       </c>
       <c r="B17" s="23" t="str">
-        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E37,CÁLCULOS!A17-1),"-")</f>
+        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E38,CÁLCULOS!A17-1),"-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
-        <f>'COM FÓRMULAS'!D38*'COM FÓRMULAS'!G38</f>
+        <f>'COM FÓRMULAS'!D39*'COM FÓRMULAS'!G39</f>
         <v>0</v>
       </c>
       <c r="B18" s="23" t="str">
-        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E38,CÁLCULOS!A18-1),"-")</f>
+        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E39,CÁLCULOS!A18-1),"-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
-        <f>'COM FÓRMULAS'!D39*'COM FÓRMULAS'!G39</f>
+        <f>'COM FÓRMULAS'!D40*'COM FÓRMULAS'!G40</f>
         <v>0</v>
       </c>
       <c r="B19" s="23" t="str">
-        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E39,CÁLCULOS!A19-1),"-")</f>
+        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E40,CÁLCULOS!A19-1),"-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
-        <f>'COM FÓRMULAS'!D40*'COM FÓRMULAS'!G40</f>
+        <f>'COM FÓRMULAS'!D41*'COM FÓRMULAS'!G41</f>
         <v>0</v>
       </c>
       <c r="B20" s="23" t="str">
-        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E40,CÁLCULOS!A20-1),"-")</f>
+        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E41,CÁLCULOS!A20-1),"-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
-        <f>'COM FÓRMULAS'!D41*'COM FÓRMULAS'!G41</f>
+        <f>'COM FÓRMULAS'!D42*'COM FÓRMULAS'!G42</f>
         <v>0</v>
       </c>
       <c r="B21" s="23" t="str">
-        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E41,CÁLCULOS!A21-1),"-")</f>
+        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E42,CÁLCULOS!A21-1),"-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
-        <f>'COM FÓRMULAS'!D42*'COM FÓRMULAS'!G42</f>
+        <f>'COM FÓRMULAS'!D43*'COM FÓRMULAS'!G43</f>
         <v>0</v>
       </c>
       <c r="B22" s="23" t="str">
-        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E42,CÁLCULOS!A22-1),"-")</f>
+        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E43,CÁLCULOS!A22-1),"-")</f>
         <v>-</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizando Gráfico de GANTT, planilha de UAT, BackLog e documentos de layouts
</commit_message>
<xml_diff>
--- a/Documentação/Gráficos/Gráfico de GANTT.xlsx
+++ b/Documentação/Gráficos/Gráfico de GANTT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITHUB\Documentos\Documentação\Gráficos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D706C741-F2F6-4CF0-ABC9-8BB247A807C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7ED46E51-F75A-4DF9-A86B-7F4FBBB9005F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="461" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>#</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>Implementação de fila</t>
+  </si>
+  <si>
+    <t>White Paper do projeto</t>
   </si>
 </sst>
 </file>
@@ -1037,7 +1040,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.33333333333333331</c:v>
+                  <c:v>0.73529411764705888</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3111,13 +3114,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:EQ36"/>
+  <dimension ref="A1:EQ37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="8" topLeftCell="H27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="8" topLeftCell="BC24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C31" sqref="C31"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3172,22 +3175,22 @@
       <c r="E5" s="34"/>
       <c r="F5" s="37">
         <f ca="1">TODAY()</f>
-        <v>44689</v>
+        <v>44702</v>
       </c>
       <c r="G5" s="37"/>
     </row>
     <row r="6" spans="1:147" s="2" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="27">
-        <f>(SUM(CÁLCULOS!A3:A22)/SUM('COM FÓRMULAS'!D9:D32))</f>
-        <v>0.33333333333333331</v>
+        <f>(SUM(CÁLCULOS!A3:A22)/SUM('COM FÓRMULAS'!D9:D19))</f>
+        <v>0.73529411764705888</v>
       </c>
       <c r="D6" s="35" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="35"/>
       <c r="F6" s="38">
-        <f>(F32-E9)+1</f>
-        <v>54</v>
+        <f>(F33-E9)+0</f>
+        <v>60</v>
       </c>
       <c r="G6" s="38"/>
     </row>
@@ -5759,7 +5762,7 @@
         <v>44669</v>
       </c>
       <c r="F20" s="13">
-        <f t="shared" ref="F20:F32" si="103">WORKDAY(E20,(D20-1))</f>
+        <f t="shared" ref="F20:F33" si="103">WORKDAY(E20,(D20-1))</f>
         <v>44670</v>
       </c>
       <c r="G20" s="10">
@@ -5924,7 +5927,7 @@
         <v>44687</v>
       </c>
       <c r="G21" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" s="19"/>
       <c r="I21" s="19"/>
@@ -6078,14 +6081,14 @@
         <v>1</v>
       </c>
       <c r="E22" s="9">
-        <v>44688</v>
+        <v>44689</v>
       </c>
       <c r="F22" s="13">
         <f t="shared" si="103"/>
-        <v>44688</v>
+        <v>44689</v>
       </c>
       <c r="G22" s="10">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H22" s="19"/>
       <c r="I22" s="19"/>
@@ -6239,14 +6242,14 @@
         <v>1</v>
       </c>
       <c r="E23" s="9">
-        <v>44688</v>
+        <v>44690</v>
       </c>
       <c r="F23" s="13">
         <f t="shared" si="103"/>
-        <v>44688</v>
+        <v>44690</v>
       </c>
       <c r="G23" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" s="19"/>
       <c r="I23" s="19"/>
@@ -6400,14 +6403,14 @@
         <v>1</v>
       </c>
       <c r="E24" s="9">
-        <v>44688</v>
+        <v>44692</v>
       </c>
       <c r="F24" s="13">
         <f t="shared" si="103"/>
-        <v>44688</v>
+        <v>44692</v>
       </c>
       <c r="G24" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24" s="19"/>
       <c r="I24" s="19"/>
@@ -6561,14 +6564,14 @@
         <v>1</v>
       </c>
       <c r="E25" s="9">
-        <v>44689</v>
+        <v>44693</v>
       </c>
       <c r="F25" s="13">
         <f t="shared" si="103"/>
-        <v>44689</v>
+        <v>44693</v>
       </c>
       <c r="G25" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25" s="19"/>
       <c r="I25" s="19"/>
@@ -6722,11 +6725,11 @@
         <v>1</v>
       </c>
       <c r="E26" s="9">
-        <v>44690</v>
+        <v>44695</v>
       </c>
       <c r="F26" s="13">
         <f t="shared" si="103"/>
-        <v>44690</v>
+        <v>44695</v>
       </c>
       <c r="G26" s="10">
         <v>0.5</v>
@@ -6883,14 +6886,14 @@
         <v>1</v>
       </c>
       <c r="E27" s="9">
-        <v>44692</v>
+        <v>44697</v>
       </c>
       <c r="F27" s="13">
         <f t="shared" si="103"/>
-        <v>44692</v>
+        <v>44697</v>
       </c>
       <c r="G27" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27" s="19"/>
       <c r="I27" s="19"/>
@@ -7051,7 +7054,7 @@
         <v>44693</v>
       </c>
       <c r="G28" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28" s="19"/>
       <c r="I28" s="19"/>
@@ -7212,7 +7215,7 @@
         <v>44697</v>
       </c>
       <c r="G29" s="10">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H29" s="19"/>
       <c r="I29" s="19"/>
@@ -7363,17 +7366,17 @@
         <v>21</v>
       </c>
       <c r="D30" s="26">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E30" s="9">
         <v>44695</v>
       </c>
       <c r="F30" s="13">
         <f t="shared" si="103"/>
-        <v>44698</v>
+        <v>44700</v>
       </c>
       <c r="G30" s="10">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H30" s="19"/>
       <c r="I30" s="19"/>
@@ -7524,14 +7527,14 @@
         <v>27</v>
       </c>
       <c r="D31" s="26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E31" s="9">
-        <v>44696</v>
+        <v>44697</v>
       </c>
       <c r="F31" s="13">
         <f t="shared" si="103"/>
-        <v>44698</v>
+        <v>44700</v>
       </c>
       <c r="G31" s="10">
         <v>0</v>
@@ -7682,17 +7685,17 @@
         <v>24</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D32" s="26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E32" s="9">
-        <v>44698</v>
+        <v>44703</v>
       </c>
       <c r="F32" s="13">
         <f t="shared" si="103"/>
-        <v>44698</v>
+        <v>44704</v>
       </c>
       <c r="G32" s="10">
         <v>0</v>
@@ -7838,26 +7841,175 @@
       <c r="EP32" s="19"/>
       <c r="EQ32" s="19"/>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C35" s="1"/>
+    <row r="33" spans="2:147" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="7">
+        <v>25</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33" s="26">
+        <v>2</v>
+      </c>
+      <c r="E33" s="9">
+        <v>44704</v>
+      </c>
+      <c r="F33" s="13">
+        <f t="shared" si="103"/>
+        <v>44705</v>
+      </c>
+      <c r="G33" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
+      <c r="L33" s="19"/>
+      <c r="M33" s="19"/>
+      <c r="N33" s="19"/>
+      <c r="O33" s="19"/>
+      <c r="P33" s="19"/>
+      <c r="Q33" s="19"/>
+      <c r="R33" s="19"/>
+      <c r="S33" s="19"/>
+      <c r="T33" s="19"/>
+      <c r="U33" s="19"/>
+      <c r="V33" s="19"/>
+      <c r="W33" s="19"/>
+      <c r="X33" s="19"/>
+      <c r="Y33" s="19"/>
+      <c r="Z33" s="19"/>
+      <c r="AA33" s="19"/>
+      <c r="AB33" s="19"/>
+      <c r="AC33" s="19"/>
+      <c r="AD33" s="19"/>
+      <c r="AE33" s="19"/>
+      <c r="AF33" s="19"/>
+      <c r="AG33" s="19"/>
+      <c r="AH33" s="19"/>
+      <c r="AI33" s="19"/>
+      <c r="AJ33" s="19"/>
+      <c r="AK33" s="19"/>
+      <c r="AL33" s="19"/>
+      <c r="AM33" s="19"/>
+      <c r="AN33" s="19"/>
+      <c r="AO33" s="19"/>
+      <c r="AP33" s="19"/>
+      <c r="AQ33" s="19"/>
+      <c r="AR33" s="19"/>
+      <c r="AS33" s="19"/>
+      <c r="AT33" s="19"/>
+      <c r="AU33" s="19"/>
+      <c r="AV33" s="19"/>
+      <c r="AW33" s="19"/>
+      <c r="AX33" s="19"/>
+      <c r="AY33" s="19"/>
+      <c r="AZ33" s="19"/>
+      <c r="BA33" s="19"/>
+      <c r="BB33" s="19"/>
+      <c r="BC33" s="19"/>
+      <c r="BD33" s="19"/>
+      <c r="BE33" s="19"/>
+      <c r="BF33" s="19"/>
+      <c r="BG33" s="19"/>
+      <c r="BH33" s="19"/>
+      <c r="BI33" s="19"/>
+      <c r="BJ33" s="19"/>
+      <c r="BK33" s="19"/>
+      <c r="BL33" s="19"/>
+      <c r="BM33" s="19"/>
+      <c r="BN33" s="19"/>
+      <c r="BO33" s="19"/>
+      <c r="BP33" s="19"/>
+      <c r="BQ33" s="19"/>
+      <c r="BR33" s="19"/>
+      <c r="BS33" s="19"/>
+      <c r="BT33" s="19"/>
+      <c r="BU33" s="19"/>
+      <c r="BV33" s="19"/>
+      <c r="BW33" s="19"/>
+      <c r="BX33" s="19"/>
+      <c r="BY33" s="19"/>
+      <c r="BZ33" s="19"/>
+      <c r="CA33" s="19"/>
+      <c r="CB33" s="19"/>
+      <c r="CC33" s="19"/>
+      <c r="CD33" s="19"/>
+      <c r="CE33" s="19"/>
+      <c r="CF33" s="19"/>
+      <c r="CG33" s="19"/>
+      <c r="CH33" s="19"/>
+      <c r="CI33" s="19"/>
+      <c r="CJ33" s="19"/>
+      <c r="CK33" s="19"/>
+      <c r="CL33" s="19"/>
+      <c r="CM33" s="19"/>
+      <c r="CN33" s="19"/>
+      <c r="CO33" s="19"/>
+      <c r="CP33" s="19"/>
+      <c r="CQ33" s="19"/>
+      <c r="CR33" s="19"/>
+      <c r="CS33" s="19"/>
+      <c r="CT33" s="19"/>
+      <c r="CU33" s="19"/>
+      <c r="CV33" s="19"/>
+      <c r="CW33" s="19"/>
+      <c r="CX33" s="19"/>
+      <c r="CY33" s="19"/>
+      <c r="CZ33" s="19"/>
+      <c r="DA33" s="19"/>
+      <c r="DB33" s="19"/>
+      <c r="DC33" s="19"/>
+      <c r="DD33" s="19"/>
+      <c r="DE33" s="19"/>
+      <c r="DF33" s="19"/>
+      <c r="DG33" s="19"/>
+      <c r="DH33" s="19"/>
+      <c r="DI33" s="19"/>
+      <c r="DJ33" s="19"/>
+      <c r="DK33" s="19"/>
+      <c r="DL33" s="19"/>
+      <c r="DM33" s="19"/>
+      <c r="DN33" s="19"/>
+      <c r="DO33" s="19"/>
+      <c r="DP33" s="19"/>
+      <c r="DQ33" s="19"/>
+      <c r="DR33" s="19"/>
+      <c r="DS33" s="19"/>
+      <c r="DT33" s="19"/>
+      <c r="DU33" s="19"/>
+      <c r="DV33" s="19"/>
+      <c r="DW33" s="19"/>
+      <c r="DX33" s="19"/>
+      <c r="DY33" s="19"/>
+      <c r="DZ33" s="19"/>
+      <c r="EA33" s="19"/>
+      <c r="EB33" s="19"/>
+      <c r="EC33" s="19"/>
+      <c r="ED33" s="19"/>
+      <c r="EE33" s="19"/>
+      <c r="EF33" s="19"/>
+      <c r="EG33" s="19"/>
+      <c r="EH33" s="19"/>
+      <c r="EI33" s="19"/>
+      <c r="EJ33" s="19"/>
+      <c r="EK33" s="19"/>
+      <c r="EL33" s="19"/>
+      <c r="EM33" s="19"/>
+      <c r="EN33" s="19"/>
+      <c r="EO33" s="19"/>
+      <c r="EP33" s="19"/>
+      <c r="EQ33" s="19"/>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:147" x14ac:dyDescent="0.3">
       <c r="C36" s="1"/>
+    </row>
+    <row r="37" spans="2:147" x14ac:dyDescent="0.3">
+      <c r="C37" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="EK7:EQ7"/>
-    <mergeCell ref="BE7:BK7"/>
-    <mergeCell ref="BS7:BY7"/>
-    <mergeCell ref="BZ7:CF7"/>
-    <mergeCell ref="CG7:CM7"/>
-    <mergeCell ref="CN7:CT7"/>
-    <mergeCell ref="CU7:DA7"/>
-    <mergeCell ref="DB7:DH7"/>
-    <mergeCell ref="DI7:DO7"/>
-    <mergeCell ref="DP7:DV7"/>
-    <mergeCell ref="DW7:EC7"/>
-    <mergeCell ref="ED7:EJ7"/>
     <mergeCell ref="AX7:BD7"/>
     <mergeCell ref="BL7:BR7"/>
     <mergeCell ref="A1:G2"/>
@@ -7874,38 +8026,50 @@
     <mergeCell ref="AC7:AI7"/>
     <mergeCell ref="AJ7:AP7"/>
     <mergeCell ref="AQ7:AW7"/>
+    <mergeCell ref="EK7:EQ7"/>
+    <mergeCell ref="BE7:BK7"/>
+    <mergeCell ref="BS7:BY7"/>
+    <mergeCell ref="BZ7:CF7"/>
+    <mergeCell ref="CG7:CM7"/>
+    <mergeCell ref="CN7:CT7"/>
+    <mergeCell ref="CU7:DA7"/>
+    <mergeCell ref="DB7:DH7"/>
+    <mergeCell ref="DI7:DO7"/>
+    <mergeCell ref="DP7:DV7"/>
+    <mergeCell ref="DW7:EC7"/>
+    <mergeCell ref="ED7:EJ7"/>
   </mergeCells>
-  <conditionalFormatting sqref="B18:D19 B17 D17 B9:G10 B16:D16 E16:F32 B11:F15 B20:C20 G11:G32 B21:D31">
+  <conditionalFormatting sqref="B18:D19 B17 D17 B9:G10 B16:D16 E16:F33 B11:F15 B20:C20 B21:D32 G11:G33">
     <cfRule type="expression" dxfId="26" priority="21">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H9:BD31 BL9:EQ31">
+  <conditionalFormatting sqref="H9:BD32 BL9:EQ32">
     <cfRule type="expression" dxfId="25" priority="20">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H9:BD31 BL9:EQ31">
+  <conditionalFormatting sqref="H9:BD32 BL9:EQ32">
     <cfRule type="expression" dxfId="24" priority="18">
       <formula>AND(H$8&gt;=$E9,H$8&lt;=$F9)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H9:BD31 BL9:EQ31">
+  <conditionalFormatting sqref="H9:BD32 BL9:EQ32">
     <cfRule type="expression" dxfId="23" priority="19">
       <formula>OR(WEEKDAY(H$8,2)=6,WEEKDAY(H$8,2)=7)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BE9:BK31">
+  <conditionalFormatting sqref="BE9:BK32">
     <cfRule type="expression" dxfId="22" priority="16">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BE9:BK31">
+  <conditionalFormatting sqref="BE9:BK32">
     <cfRule type="expression" dxfId="21" priority="14">
       <formula>AND(BE$8&gt;=$E9,BE$8&lt;=$F9)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BE9:BK31">
+  <conditionalFormatting sqref="BE9:BK32">
     <cfRule type="expression" dxfId="20" priority="15">
       <formula>OR(WEEKDAY(BE$8,2)=6,WEEKDAY(BE$8,2)=7)</formula>
     </cfRule>
@@ -7924,37 +8088,37 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B32:D32">
+  <conditionalFormatting sqref="B33:D33">
     <cfRule type="expression" dxfId="19" priority="11">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H32:BD32 BL32:EQ32">
+  <conditionalFormatting sqref="H33:BD33 BL33:EQ33">
     <cfRule type="expression" dxfId="18" priority="10">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H32:BD32 BL32:EQ32">
+  <conditionalFormatting sqref="H33:BD33 BL33:EQ33">
     <cfRule type="expression" dxfId="17" priority="8">
-      <formula>AND(H$8&gt;=$E32,H$8&lt;=$F32)</formula>
+      <formula>AND(H$8&gt;=$E33,H$8&lt;=$F33)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H32:BD32 BL32:EQ32">
+  <conditionalFormatting sqref="H33:BD33 BL33:EQ33">
     <cfRule type="expression" dxfId="16" priority="9">
       <formula>OR(WEEKDAY(H$8,2)=6,WEEKDAY(H$8,2)=7)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BE32:BK32">
+  <conditionalFormatting sqref="BE33:BK33">
     <cfRule type="expression" dxfId="15" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BE32:BK32">
+  <conditionalFormatting sqref="BE33:BK33">
     <cfRule type="expression" dxfId="14" priority="4">
-      <formula>AND(BE$8&gt;=$E32,BE$8&lt;=$F32)</formula>
+      <formula>AND(BE$8&gt;=$E33,BE$8&lt;=$F33)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BE32:BK32">
+  <conditionalFormatting sqref="BE33:BK33">
     <cfRule type="expression" dxfId="13" priority="5">
       <formula>OR(WEEKDAY(BE$8,2)=6,WEEKDAY(BE$8,2)=7)</formula>
     </cfRule>
@@ -8005,7 +8169,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="7" id="{26BB7447-3313-4134-A3BE-8E2C5A638A34}">
-            <xm:f>AND(H$8&lt;=CÁLCULOS!$B11,H$8&gt;=$E32,CÁLCULOS!$A11&gt;=1)</xm:f>
+            <xm:f>AND(H$8&lt;=CÁLCULOS!$B11,H$8&gt;=$E33,CÁLCULOS!$A11&gt;=1)</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -8014,11 +8178,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>H32:BD32 BL32:EQ32</xm:sqref>
+          <xm:sqref>H33:BD33 BL33:EQ33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="3" id="{4896A4C4-8F9E-4217-962B-723F1989E39D}">
-            <xm:f>AND(BE$8&lt;=CÁLCULOS!$B11,BE$8&gt;=$E32,CÁLCULOS!$A11&gt;=1)</xm:f>
+            <xm:f>AND(BE$8&lt;=CÁLCULOS!$B11,BE$8&gt;=$E33,CÁLCULOS!$A11&gt;=1)</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -8027,7 +8191,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>BE32:BK32</xm:sqref>
+          <xm:sqref>BE33:BK33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="23" id="{A4E1E301-260B-439C-8FA5-07AD136299B7}">
@@ -8079,7 +8243,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>H31:EQ31</xm:sqref>
+          <xm:sqref>H31:EQ32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="47" id="{26BB7447-3313-4134-A3BE-8E2C5A638A34}">
@@ -8234,121 +8398,121 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
-        <f>'COM FÓRMULAS'!D32*'COM FÓRMULAS'!G32</f>
-        <v>0</v>
+        <f>'COM FÓRMULAS'!D33*'COM FÓRMULAS'!G33</f>
+        <v>0.5</v>
       </c>
       <c r="B11" s="23">
-        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E32,CÁLCULOS!A11-1),"-")</f>
-        <v>44697</v>
+        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E33,CÁLCULOS!A11-1),"-")</f>
+        <v>44701</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
-        <f>'COM FÓRMULAS'!D33*'COM FÓRMULAS'!G33</f>
+        <f>'COM FÓRMULAS'!D34*'COM FÓRMULAS'!G34</f>
         <v>0</v>
       </c>
       <c r="B12" s="23" t="str">
-        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E33,CÁLCULOS!A12-1),"-")</f>
+        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E34,CÁLCULOS!A12-1),"-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
-        <f>'COM FÓRMULAS'!D34*'COM FÓRMULAS'!G34</f>
+        <f>'COM FÓRMULAS'!D35*'COM FÓRMULAS'!G35</f>
         <v>0</v>
       </c>
       <c r="B13" s="23" t="str">
-        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E34,CÁLCULOS!A13-1),"-")</f>
+        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E35,CÁLCULOS!A13-1),"-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
-        <f>'COM FÓRMULAS'!D35*'COM FÓRMULAS'!G35</f>
+        <f>'COM FÓRMULAS'!D36*'COM FÓRMULAS'!G36</f>
         <v>0</v>
       </c>
       <c r="B14" s="23" t="str">
-        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E35,CÁLCULOS!A14-1),"-")</f>
+        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E36,CÁLCULOS!A14-1),"-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
-        <f>'COM FÓRMULAS'!D36*'COM FÓRMULAS'!G36</f>
+        <f>'COM FÓRMULAS'!D37*'COM FÓRMULAS'!G37</f>
         <v>0</v>
       </c>
       <c r="B15" s="23" t="str">
-        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E36,CÁLCULOS!A15-1),"-")</f>
+        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E37,CÁLCULOS!A15-1),"-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
-        <f>'COM FÓRMULAS'!D37*'COM FÓRMULAS'!G37</f>
+        <f>'COM FÓRMULAS'!D38*'COM FÓRMULAS'!G38</f>
         <v>0</v>
       </c>
       <c r="B16" s="23" t="str">
-        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E37,CÁLCULOS!A16-1),"-")</f>
+        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E38,CÁLCULOS!A16-1),"-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
-        <f>'COM FÓRMULAS'!D38*'COM FÓRMULAS'!G38</f>
+        <f>'COM FÓRMULAS'!D39*'COM FÓRMULAS'!G39</f>
         <v>0</v>
       </c>
       <c r="B17" s="23" t="str">
-        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E38,CÁLCULOS!A17-1),"-")</f>
+        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E39,CÁLCULOS!A17-1),"-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
-        <f>'COM FÓRMULAS'!D39*'COM FÓRMULAS'!G39</f>
+        <f>'COM FÓRMULAS'!D40*'COM FÓRMULAS'!G40</f>
         <v>0</v>
       </c>
       <c r="B18" s="23" t="str">
-        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E39,CÁLCULOS!A18-1),"-")</f>
+        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E40,CÁLCULOS!A18-1),"-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
-        <f>'COM FÓRMULAS'!D40*'COM FÓRMULAS'!G40</f>
+        <f>'COM FÓRMULAS'!D41*'COM FÓRMULAS'!G41</f>
         <v>0</v>
       </c>
       <c r="B19" s="23" t="str">
-        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E40,CÁLCULOS!A19-1),"-")</f>
+        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E41,CÁLCULOS!A19-1),"-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
-        <f>'COM FÓRMULAS'!D41*'COM FÓRMULAS'!G41</f>
+        <f>'COM FÓRMULAS'!D42*'COM FÓRMULAS'!G42</f>
         <v>0</v>
       </c>
       <c r="B20" s="23" t="str">
-        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E41,CÁLCULOS!A20-1),"-")</f>
+        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E42,CÁLCULOS!A20-1),"-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
-        <f>'COM FÓRMULAS'!D42*'COM FÓRMULAS'!G42</f>
+        <f>'COM FÓRMULAS'!D43*'COM FÓRMULAS'!G43</f>
         <v>0</v>
       </c>
       <c r="B21" s="23" t="str">
-        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E42,CÁLCULOS!A21-1),"-")</f>
+        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E43,CÁLCULOS!A21-1),"-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
-        <f>'COM FÓRMULAS'!D43*'COM FÓRMULAS'!G43</f>
+        <f>'COM FÓRMULAS'!D44*'COM FÓRMULAS'!G44</f>
         <v>0</v>
       </c>
       <c r="B22" s="23" t="str">
-        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E43,CÁLCULOS!A22-1),"-")</f>
+        <f>IFERROR(WORKDAY('COM FÓRMULAS'!E44,CÁLCULOS!A22-1),"-")</f>
         <v>-</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Subindo White Paper finalizado e organização dos diretórios
</commit_message>
<xml_diff>
--- a/Documentação/Gráficos/Gráfico de GANTT.xlsx
+++ b/Documentação/Gráficos/Gráfico de GANTT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITHUB\Documentos\Documentação\Gráficos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7ED46E51-F75A-4DF9-A86B-7F4FBBB9005F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA0ED1A-B223-443A-8B76-C53D75C2F97B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="461" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1040,7 +1040,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.73529411764705888</c:v>
+                  <c:v>0.875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3117,10 +3117,10 @@
   <dimension ref="A1:EQ37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="8" topLeftCell="BC24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="8" topLeftCell="BC30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3175,14 +3175,14 @@
       <c r="E5" s="34"/>
       <c r="F5" s="37">
         <f ca="1">TODAY()</f>
-        <v>44702</v>
+        <v>44709</v>
       </c>
       <c r="G5" s="37"/>
     </row>
     <row r="6" spans="1:147" s="2" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="27">
-        <f>(SUM(CÁLCULOS!A3:A22)/SUM('COM FÓRMULAS'!D9:D19))</f>
-        <v>0.73529411764705888</v>
+        <f>(SUM(CÁLCULOS!A3:A22)/SUM('COM FÓRMULAS'!D9:D18))</f>
+        <v>0.875</v>
       </c>
       <c r="D6" s="35" t="s">
         <v>7</v>
@@ -7376,7 +7376,7 @@
         <v>44700</v>
       </c>
       <c r="G30" s="10">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H30" s="19"/>
       <c r="I30" s="19"/>
@@ -7698,7 +7698,7 @@
         <v>44704</v>
       </c>
       <c r="G32" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32" s="19"/>
       <c r="I32" s="19"/>
@@ -7859,7 +7859,7 @@
         <v>44705</v>
       </c>
       <c r="G33" s="10">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="H33" s="19"/>
       <c r="I33" s="19"/>
@@ -8010,6 +8010,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="EK7:EQ7"/>
+    <mergeCell ref="BE7:BK7"/>
+    <mergeCell ref="BS7:BY7"/>
+    <mergeCell ref="BZ7:CF7"/>
+    <mergeCell ref="CG7:CM7"/>
+    <mergeCell ref="CN7:CT7"/>
+    <mergeCell ref="CU7:DA7"/>
+    <mergeCell ref="DB7:DH7"/>
+    <mergeCell ref="DI7:DO7"/>
+    <mergeCell ref="DP7:DV7"/>
+    <mergeCell ref="DW7:EC7"/>
+    <mergeCell ref="ED7:EJ7"/>
     <mergeCell ref="AX7:BD7"/>
     <mergeCell ref="BL7:BR7"/>
     <mergeCell ref="A1:G2"/>
@@ -8026,18 +8038,6 @@
     <mergeCell ref="AC7:AI7"/>
     <mergeCell ref="AJ7:AP7"/>
     <mergeCell ref="AQ7:AW7"/>
-    <mergeCell ref="EK7:EQ7"/>
-    <mergeCell ref="BE7:BK7"/>
-    <mergeCell ref="BS7:BY7"/>
-    <mergeCell ref="BZ7:CF7"/>
-    <mergeCell ref="CG7:CM7"/>
-    <mergeCell ref="CN7:CT7"/>
-    <mergeCell ref="CU7:DA7"/>
-    <mergeCell ref="DB7:DH7"/>
-    <mergeCell ref="DI7:DO7"/>
-    <mergeCell ref="DP7:DV7"/>
-    <mergeCell ref="DW7:EC7"/>
-    <mergeCell ref="ED7:EJ7"/>
   </mergeCells>
   <conditionalFormatting sqref="B18:D19 B17 D17 B9:G10 B16:D16 E16:F33 B11:F15 B20:C20 B21:D32 G11:G33">
     <cfRule type="expression" dxfId="26" priority="21">
@@ -8399,11 +8399,11 @@
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>'COM FÓRMULAS'!D33*'COM FÓRMULAS'!G33</f>
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="B11" s="23">
         <f>IFERROR(WORKDAY('COM FÓRMULAS'!E33,CÁLCULOS!A11-1),"-")</f>
-        <v>44701</v>
+        <v>44705</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>